<commit_message>
Adding materials for retrofit analysis. These new materials are reflected in the GenericHome-base, GenericHome-2storey and GenericHome-3storey databases.
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
@@ -756,7 +756,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +791,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1">
-        <v>285.3</v>
+        <v>264.3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -804,7 +804,7 @@
       </c>
       <c r="H2">
         <f>+(B26-B25)*(D31-D26)</f>
-        <v>29.723860960514532</v>
+        <v>35.038745320002533</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
@@ -816,7 +816,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" t="s">
@@ -827,7 +827,7 @@
       </c>
       <c r="H3">
         <f>+(C27-C26)*(D31-D27)</f>
-        <v>29.723860960514532</v>
+        <v>35.038745320002533</v>
       </c>
       <c r="I3" t="s">
         <v>3</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="C4" s="13">
         <f>+$C$2/C3</f>
-        <v>95.100000000000009</v>
+        <v>132.15</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>3</v>
@@ -855,7 +855,7 @@
       </c>
       <c r="H4">
         <f>+(B27-B28)*(D31-D28)</f>
-        <v>29.723860960514532</v>
+        <v>35.038745320002533</v>
       </c>
       <c r="I4" t="s">
         <v>3</v>
@@ -870,7 +870,7 @@
       </c>
       <c r="C5" s="2">
         <f>+SQRT(C4)</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -883,7 +883,7 @@
       </c>
       <c r="H5">
         <f>+(C28-C25)*(D32-D28)</f>
-        <v>29.723860960514532</v>
+        <v>35.038745320002533</v>
       </c>
       <c r="I5" t="s">
         <v>3</v>
@@ -898,7 +898,7 @@
       </c>
       <c r="C6" s="2">
         <f>+SQRT(C4)</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -912,7 +912,7 @@
       </c>
       <c r="H6">
         <f>+(B30*C31)</f>
-        <v>95.100000000000009</v>
+        <v>132.15</v>
       </c>
       <c r="I6" t="s">
         <v>3</v>
@@ -937,7 +937,7 @@
       </c>
       <c r="H7">
         <f>+C28*B27</f>
-        <v>95.100000000000009</v>
+        <v>132.15</v>
       </c>
       <c r="I7" t="s">
         <v>3</v>
@@ -970,14 +970,14 @@
       </c>
       <c r="H8" s="15">
         <f>+H2*$C$7/100</f>
-        <v>4.4585791440771798</v>
+        <v>5.2558117980003791</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="J8" s="19">
         <f>+H8/K8</f>
-        <v>2.9255768661923756</v>
+        <v>3.4486954055120602</v>
       </c>
       <c r="K8" s="9">
         <f>+($C$10-$C$8)/2</f>
@@ -1003,14 +1003,14 @@
       </c>
       <c r="H9" s="16">
         <f>+H3*$C$7/100</f>
-        <v>4.4585791440771798</v>
+        <v>5.2558117980003791</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="20">
         <f t="shared" ref="J9" si="0">+H9/K9</f>
-        <v>2.9255768661923756</v>
+        <v>3.4486954055120602</v>
       </c>
       <c r="K9" s="11">
         <f>+($C$10-$C$8)/2</f>
@@ -1039,14 +1039,14 @@
       </c>
       <c r="H10" s="17">
         <f>+H4*$C$7/100</f>
-        <v>4.4585791440771798</v>
+        <v>5.2558117980003791</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J10" s="21">
         <f>+H10/K10</f>
-        <v>2.9255768661923756</v>
+        <v>3.4486954055120602</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" ref="K10:K11" si="1">+($C$10-$C$8)/2</f>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="C11" s="13">
         <f>+C5/2</f>
-        <v>4.8759614436539591</v>
+        <v>5.7478256758534352</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>6</v>
@@ -1073,14 +1073,14 @@
       </c>
       <c r="H11" s="18">
         <f>+H5*$C$7/100</f>
-        <v>4.4585791440771798</v>
+        <v>5.2558117980003791</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J11" s="22">
         <f>+H11/K11</f>
-        <v>2.9255768661923756</v>
+        <v>3.4486954055120602</v>
       </c>
       <c r="K11" s="14">
         <f t="shared" si="1"/>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="C15" s="15">
         <f>+$B$34</f>
-        <v>3.4255768661923756</v>
+        <v>3.9486954055120602</v>
       </c>
       <c r="F15" t="s">
         <v>78</v>
@@ -1150,8 +1150,8 @@
         <v>80</v>
       </c>
       <c r="H15" s="23">
-        <f>10.363+($C$5*H14)</f>
-        <v>16.864281924871946</v>
+        <f>7.9248+($C$5*H14)</f>
+        <v>15.588567567804581</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>6</v>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C17" s="16">
         <f>+$C$38</f>
-        <v>3.4255768661923756</v>
+        <v>3.9486954055120602</v>
       </c>
       <c r="F17" t="s">
         <v>79</v>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="C18" s="17">
         <f>+$B$41</f>
-        <v>9.2519228873079182</v>
+        <v>10.99565135170687</v>
       </c>
       <c r="F18" t="s">
         <v>78</v>
@@ -1201,8 +1201,8 @@
         <v>81</v>
       </c>
       <c r="H18" s="23">
-        <f>10.363+($C$5*H17)</f>
-        <v>11.988320481217986</v>
+        <f>7.9248+($C$5*H17)</f>
+        <v>9.8407418919511453</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>6</v>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="C19" s="17">
         <f>+$B$42</f>
-        <v>6.3263460211155422</v>
+        <v>7.5469559461948101</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="C20" s="12">
         <f>+$C$45</f>
-        <v>9.2519228873079182</v>
+        <v>10.99565135170687</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C21" s="18">
         <f>+$C$46</f>
-        <v>6.3263460211155422</v>
+        <v>7.5469559461948101</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B26" s="4">
         <f>+$C$5</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -1286,11 +1286,11 @@
       </c>
       <c r="B27" s="4">
         <f>+$C$5</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C27" s="3">
         <f>+$C$6</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D27" s="3">
         <f>+$C$8</f>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="C28" s="3">
         <f>+$C$6</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D28" s="3">
         <f>+$C$8</f>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="B30" s="4">
         <f>+$C$5</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -1350,11 +1350,11 @@
       </c>
       <c r="B31" s="4">
         <f>+$C$5</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C31" s="3">
         <f>+$C$6</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="2"/>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C32" s="3">
         <f>+$C$6</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D32" s="3">
         <f>+$C$10</f>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B34" s="19">
         <f>+B33+$J$8</f>
-        <v>3.4255768661923756</v>
+        <v>3.9486954055120602</v>
       </c>
       <c r="C34" s="9">
         <f>+C26</f>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B35" s="19">
         <f>+B33+$J$8</f>
-        <v>3.4255768661923756</v>
+        <v>3.9486954055120602</v>
       </c>
       <c r="C35" s="9">
         <f>+C29</f>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B37" s="20">
         <f>+B26</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C37" s="11">
         <f>+C26+0.5</f>
@@ -1468,11 +1468,11 @@
       </c>
       <c r="B38" s="20">
         <f>+B27</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C38" s="11">
         <f>+C37+J9</f>
-        <v>3.4255768661923756</v>
+        <v>3.9486954055120602</v>
       </c>
       <c r="D38" s="11">
         <f>+D27+0.5</f>
@@ -1485,11 +1485,11 @@
       </c>
       <c r="B39" s="20">
         <f>+B31</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C39" s="11">
         <f>+C37+$J$9</f>
-        <v>3.4255768661923756</v>
+        <v>3.9486954055120602</v>
       </c>
       <c r="D39" s="11">
         <f>+D37+$K$9</f>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B40" s="20">
         <f>+B30</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="C40" s="11">
         <f>+C30+0.5</f>
@@ -1519,11 +1519,11 @@
       </c>
       <c r="B41" s="21">
         <f>+B27-0.5</f>
-        <v>9.2519228873079182</v>
+        <v>10.99565135170687</v>
       </c>
       <c r="C41" s="7">
         <f>+C27</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D41" s="7">
         <f>+D27+0.5</f>
@@ -1536,11 +1536,11 @@
       </c>
       <c r="B42" s="21">
         <f>+B41-$J$10</f>
-        <v>6.3263460211155422</v>
+        <v>7.5469559461948101</v>
       </c>
       <c r="C42" s="7">
         <f>+C28</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D42" s="7">
         <f>+D28+0.5</f>
@@ -1553,11 +1553,11 @@
       </c>
       <c r="B43" s="21">
         <f>+B42</f>
-        <v>6.3263460211155422</v>
+        <v>7.5469559461948101</v>
       </c>
       <c r="C43" s="7">
         <f>+C42</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D43" s="7">
         <f>+D42+$K$10</f>
@@ -1570,11 +1570,11 @@
       </c>
       <c r="B44" s="21">
         <f>+B41</f>
-        <v>9.2519228873079182</v>
+        <v>10.99565135170687</v>
       </c>
       <c r="C44" s="7">
         <f>+C43</f>
-        <v>9.7519228873079182</v>
+        <v>11.49565135170687</v>
       </c>
       <c r="D44" s="7">
         <f>+D43</f>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C45" s="14">
         <f>+C28-0.5</f>
-        <v>9.2519228873079182</v>
+        <v>10.99565135170687</v>
       </c>
       <c r="D45" s="14">
         <f>+D28+0.5</f>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="C46" s="14">
         <f>+C45-$J$11</f>
-        <v>6.3263460211155422</v>
+        <v>7.5469559461948101</v>
       </c>
       <c r="D46" s="14">
         <f>+D25+0.5</f>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="C47" s="14">
         <f>+C46</f>
-        <v>6.3263460211155422</v>
+        <v>7.5469559461948101</v>
       </c>
       <c r="D47" s="14">
         <f>+D46+$K$11</f>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="C48" s="14">
         <f>+C45</f>
-        <v>9.2519228873079182</v>
+        <v>10.99565135170687</v>
       </c>
       <c r="D48" s="14">
         <f>+D47</f>

</xml_diff>

<commit_message>
Added missing cell names
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="-15" windowWidth="15030" windowHeight="14325"/>
+    <workbookView xWindow="13980" yWindow="-15" windowWidth="14835" windowHeight="14325"/>
   </bookViews>
   <sheets>
     <sheet name="geometry calculation" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,10 @@
     <definedName name="Hght_WinWall2">'geometry calculation'!$K$10</definedName>
     <definedName name="Hght_WinWall3">'geometry calculation'!$K$11</definedName>
     <definedName name="Hght_WinWall4">'geometry calculation'!$K$12</definedName>
+    <definedName name="Len_WinWall1">'geometry calculation'!$J$9</definedName>
+    <definedName name="Len_WinWall2">'geometry calculation'!$J$10</definedName>
+    <definedName name="Len_WinWall3">'geometry calculation'!$J$11</definedName>
+    <definedName name="Len_WinWall4">'geometry calculation'!$J$12</definedName>
     <definedName name="NumStoreys" comment="Number of storeys above grade">'geometry calculation'!$C$3</definedName>
     <definedName name="Opt_Area" comment="Flor area per storey">'geometry calculation'!$C$4</definedName>
     <definedName name="Opt_Bsm_Depth" comment="Basement depth below grade">'geometry calculation'!$C$11</definedName>
@@ -37,7 +41,7 @@
     <definedName name="Opt_Roof_Peak_W">'geometry calculation'!$C$13</definedName>
     <definedName name="Opt_Width" comment="Width of first floor plan (footprint width)">'geometry calculation'!$C$5</definedName>
     <definedName name="Roof_Slope1">'geometry calculation'!$H$15</definedName>
-    <definedName name="Roof_Slope2">'geometry calculation'!$H$18</definedName>
+    <definedName name="Roof_Slope2">'geometry calculation'!#REF!</definedName>
     <definedName name="win_bottom">'geometry calculation'!$C$14</definedName>
     <definedName name="win_top">'geometry calculation'!$C$15</definedName>
     <definedName name="win_wall_1_left">'geometry calculation'!$C$17</definedName>
@@ -93,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
   <si>
     <t>%</t>
   </si>
@@ -302,15 +306,6 @@
     <t>&lt;Opt-Bsm-Depth&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;Opt-Width&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;Opt-Length&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;Opt-Roof-Peak-W&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;Opt-Roof-Height&gt;</t>
   </si>
   <si>
@@ -320,9 +315,6 @@
     <t>8/12</t>
   </si>
   <si>
-    <t>3/12</t>
-  </si>
-  <si>
     <t>Window Geometry Calculations</t>
   </si>
   <si>
@@ -360,6 +352,24 @@
   </si>
   <si>
     <t>Window height</t>
+  </si>
+  <si>
+    <t>&lt;Opt-Roof-Peak-W&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Opt-Width&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Opt-Length&gt;</t>
+  </si>
+  <si>
+    <t>Floor 1</t>
+  </si>
+  <si>
+    <t>(Ground)</t>
+  </si>
+  <si>
+    <t>Floor 1 (Ground)</t>
   </si>
 </sst>
 </file>
@@ -370,7 +380,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +448,22 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -502,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,6 +595,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,16 +909,16 @@
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="9" max="9" width="6.5703125" customWidth="1"/>
     <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>76</v>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>72</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -898,7 +926,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="23">
@@ -907,11 +935,14 @@
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="F2" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>48</v>
@@ -919,13 +950,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="22">
         <v>2</v>
       </c>
       <c r="D3" s="1"/>
+      <c r="E3" s="41" t="s">
+        <v>89</v>
+      </c>
       <c r="F3" t="s">
         <v>42</v>
       </c>
@@ -934,7 +968,7 @@
       </c>
       <c r="H3" s="35">
         <f>+(INDEX(x,2)-INDEX(x,1))*(INDEX(z,7)-INDEX(z,2))</f>
-        <v>32.170481277096236</v>
+        <v>29.447389357971954</v>
       </c>
       <c r="I3" t="s">
         <v>1</v>
@@ -942,7 +976,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -962,7 +996,7 @@
       </c>
       <c r="H4" s="35">
         <f>+(INDEX(y,3)-INDEX(y,2))*(INDEX(z,7)-(INDEX(z,3)))</f>
-        <v>32.170481277096236</v>
+        <v>29.447389357971954</v>
       </c>
       <c r="I4" t="s">
         <v>1</v>
@@ -973,7 +1007,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C5" s="12">
         <f>+SQRT(Opt_Area)</f>
@@ -990,7 +1024,7 @@
       </c>
       <c r="H5" s="35">
         <f>(INDEX(x,3)-INDEX(x,4))*(INDEX(z,7)-INDEX(z,4))</f>
-        <v>32.170481277096236</v>
+        <v>29.447389357971954</v>
       </c>
       <c r="I5" t="s">
         <v>1</v>
@@ -1001,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C6" s="12">
         <f>+SQRT(Opt_Area)</f>
@@ -1019,7 +1053,7 @@
       </c>
       <c r="H6" s="35">
         <f>(INDEX(y,4)-INDEX(y,1))*(INDEX(z,8)-INDEX(z,4))</f>
-        <v>32.170481277096236</v>
+        <v>29.447389357971954</v>
       </c>
       <c r="I6" t="s">
         <v>1</v>
@@ -1027,7 +1061,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="24">
@@ -1052,11 +1086,11 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="24">
-        <v>3.048</v>
+        <v>2.79</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>4</v>
@@ -1075,15 +1109,15 @@
         <v>1</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="24">
@@ -1100,18 +1134,18 @@
       </c>
       <c r="H9" s="16">
         <f>AreaWall1*WinAreaRatio/100</f>
-        <v>4.5038673787934735</v>
+        <v>4.1226345101160735</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J9" s="29">
         <f>AreaWinWall1/Hght_WinWall1</f>
-        <v>2.9552935556387627</v>
+        <v>2.9552935556387623</v>
       </c>
       <c r="K9" s="28">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.395</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1122,7 +1156,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="25">
-        <v>2.4384000000000001</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>4</v>
@@ -1135,29 +1169,29 @@
       </c>
       <c r="H10" s="18">
         <f>AreaWall2*WinAreaRatio/100</f>
-        <v>4.5038673787934735</v>
+        <v>4.1226345101160735</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="30">
         <f>AreaWinWall2/Hght_WinWall2</f>
-        <v>2.9552935556387627</v>
+        <v>2.9552935556387623</v>
       </c>
       <c r="K10" s="31">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.395</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C11" s="25">
-        <v>2</v>
+        <v>1.98</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>4</v>
@@ -1170,30 +1204,30 @@
       </c>
       <c r="H11" s="19">
         <f>AreaWall3*WinAreaRatio/100</f>
-        <v>4.5038673787934735</v>
+        <v>4.1226345101160735</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J11" s="32">
         <f>AreaWinWall3/Hght_WinWall3</f>
-        <v>2.9552935556387627</v>
+        <v>2.9552935556387623</v>
       </c>
       <c r="K11" s="33">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.395</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="11">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>5.4863999999999997</v>
+        <v>5.3</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>52</v>
@@ -1203,24 +1237,24 @@
       </c>
       <c r="H12" s="21">
         <f>AreaWall4*WinAreaRatio/100</f>
-        <v>4.5038673787934735</v>
+        <v>4.1226345101160735</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="J12" s="38">
         <f>AreaWinWall4/Hght_WinWall4</f>
-        <v>2.9552935556387627</v>
+        <v>2.9552935556387623</v>
       </c>
       <c r="K12" s="34">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.395</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="7" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C13" s="11">
         <f>Opt_Width/2</f>
@@ -1234,7 +1268,7 @@
       </c>
       <c r="C14" s="15">
         <f>INDEX(z,10)</f>
-        <v>2.9384000000000001</v>
+        <v>3.01</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="4"/>
@@ -1251,13 +1285,13 @@
       </c>
       <c r="C15" s="15">
         <f>INDEX(z,12)</f>
-        <v>4.4623999999999997</v>
+        <v>4.4049999999999994</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H15" s="36">
         <f>8/12</f>
@@ -1274,30 +1308,30 @@
         <v>0.5</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H16" s="37">
         <f>Opt_Main_Height+Hght_Flr2+(Opt_Width*Roof_Slope1)</f>
-        <v>14.962813227711338</v>
+        <v>14.776413227711339</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="16">
         <f>INDEX(x,10)</f>
-        <v>3.4552935556387627</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.4552935556387623</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="4" t="s">
         <v>60</v>
@@ -1306,40 +1340,17 @@
         <f>INDEX(y,13)</f>
         <v>0.5</v>
       </c>
-      <c r="F18" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="36">
-        <f>2/12</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C19" s="18">
         <f>INDEX(y,14)</f>
-        <v>3.4552935556387627</v>
-      </c>
-      <c r="F19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="37">
-        <f>Opt_Main_Height+Hght_Flr2+(Opt_Width*Roof_Slope2)</f>
-        <v>9.6855033069278349</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.4552935556387623</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>64</v>
       </c>
@@ -1348,7 +1359,7 @@
         <v>10.054619841567009</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>65</v>
       </c>
@@ -1357,7 +1368,7 @@
         <v>7.099326285928246</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>66</v>
       </c>
@@ -1366,7 +1377,7 @@
         <v>10.054619841567009</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>67</v>
       </c>
@@ -1375,7 +1386,16 @@
         <v>7.099326285928246</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>57</v>
       </c>
@@ -1389,7 +1409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1400,44 +1420,44 @@
         <v>0</v>
       </c>
       <c r="D27" s="26">
-        <f>+$C$10</f>
-        <v>2.4384000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <f>Opt_Bsm_Height</f>
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="27">
-        <f>+$C$5</f>
+        <f>Opt_Width</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C28" s="26">
         <v>0</v>
       </c>
       <c r="D28" s="26">
-        <f>+$C$10</f>
-        <v>2.4384000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <f>Opt_Bsm_Height</f>
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="27">
-        <f>+$C$5</f>
+        <f>Opt_Width</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C29" s="26">
-        <f>+$C$6</f>
+        <f>Opt_Length</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D29" s="26">
-        <f>+$C$10</f>
-        <v>2.4384000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <f>Opt_Bsm_Height</f>
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1445,15 +1465,15 @@
         <v>0</v>
       </c>
       <c r="C30" s="26">
-        <f>+$C$6</f>
+        <f>Opt_Length</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D30" s="26">
-        <f>+$C$10</f>
-        <v>2.4384000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <f>Opt_Bsm_Height</f>
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1464,24 +1484,24 @@
         <v>0</v>
       </c>
       <c r="D31" s="26">
-        <f>+$C$12</f>
-        <v>5.4863999999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <f>Opt_Main_Height</f>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="27">
-        <f>+$C$5</f>
+        <f>Opt_Width</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C32" s="26">
         <v>0</v>
       </c>
       <c r="D32" s="26">
-        <f t="shared" ref="D32:D33" si="0">+$C$12</f>
-        <v>5.4863999999999997</v>
+        <f>Opt_Main_Height</f>
+        <v>5.3</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,16 +1509,16 @@
         <v>16</v>
       </c>
       <c r="B33" s="27">
-        <f>+$C$5</f>
+        <f>Opt_Width</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C33" s="26">
-        <f>+$C$6</f>
+        <f>Opt_Length</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D33" s="26">
-        <f t="shared" si="0"/>
-        <v>5.4863999999999997</v>
+        <f>Opt_Main_Height</f>
+        <v>5.3</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,12 +1529,12 @@
         <v>0</v>
       </c>
       <c r="C34" s="26">
-        <f>+$C$6</f>
+        <f>Opt_Length</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D34" s="26">
-        <f>+$C$12</f>
-        <v>5.4863999999999997</v>
+        <f>Opt_Main_Height</f>
+        <v>5.3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,16 +1542,16 @@
         <v>18</v>
       </c>
       <c r="B35" s="28">
-        <f>+B27+0.5</f>
+        <f>INDEX(x,1)+0.5</f>
         <v>0.5</v>
       </c>
       <c r="C35" s="28">
-        <f>+C27</f>
+        <f>INDEX(y,1)</f>
         <v>0</v>
       </c>
       <c r="D35" s="28">
-        <f>+$D$27+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,1)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1539,16 +1559,16 @@
         <v>19</v>
       </c>
       <c r="B36" s="29">
-        <f>+B35+$J$9</f>
-        <v>3.4552935556387627</v>
+        <f>INDEX(x,9)+Len_WinWall1</f>
+        <v>3.4552935556387623</v>
       </c>
       <c r="C36" s="28">
-        <f>+C28</f>
+        <f>INDEX(y,2)</f>
         <v>0</v>
       </c>
       <c r="D36" s="28">
-        <f>+$D$27+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,1)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1556,16 +1576,16 @@
         <v>20</v>
       </c>
       <c r="B37" s="29">
-        <f>+B35+$J$9</f>
-        <v>3.4552935556387627</v>
+        <f>INDEX(x,9)+Len_WinWall1</f>
+        <v>3.4552935556387623</v>
       </c>
       <c r="C37" s="28">
-        <f>+C31</f>
+        <f>INDEX(y,5)</f>
         <v>0</v>
       </c>
       <c r="D37" s="28">
-        <f>+D35+$K$9</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,9)+Hght_WinWall1</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1573,16 +1593,16 @@
         <v>21</v>
       </c>
       <c r="B38" s="28">
-        <f>+B35</f>
+        <f>INDEX(x,9)</f>
         <v>0.5</v>
       </c>
       <c r="C38" s="28">
-        <f>+C32</f>
+        <f>INDEX(y,6)</f>
         <v>0</v>
       </c>
       <c r="D38" s="28">
-        <f>+D36+$K$9</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,10)+Hght_WinWall1</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,16 +1610,16 @@
         <v>22</v>
       </c>
       <c r="B39" s="30">
-        <f>+B28</f>
+        <f>INDEX(x,2)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C39" s="31">
-        <f>+C28+0.5</f>
+        <f>INDEX(y,2)+0.5</f>
         <v>0.5</v>
       </c>
       <c r="D39" s="31">
-        <f>+D28+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,2)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1607,16 +1627,16 @@
         <v>23</v>
       </c>
       <c r="B40" s="30">
-        <f>+B29</f>
+        <f>INDEX(x,3)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C40" s="31">
-        <f>+C39+J10</f>
-        <v>3.4552935556387627</v>
+        <f>INDEX(y,13)+Len_WinWall2</f>
+        <v>3.4552935556387623</v>
       </c>
       <c r="D40" s="31">
-        <f>+D29+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,3)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1624,16 +1644,16 @@
         <v>24</v>
       </c>
       <c r="B41" s="30">
-        <f>+B33</f>
+        <f>INDEX(x,7)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C41" s="31">
-        <f>+C39+$J$10</f>
-        <v>3.4552935556387627</v>
+        <f>INDEX(y,13)+Len_WinWall2</f>
+        <v>3.4552935556387623</v>
       </c>
       <c r="D41" s="31">
-        <f>+D39+$K$10</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,13)+Hght_WinWall2</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1641,16 +1661,16 @@
         <v>25</v>
       </c>
       <c r="B42" s="30">
-        <f>+B32</f>
+        <f>INDEX(x,6)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="C42" s="31">
-        <f>+C32+0.5</f>
+        <f>INDEX(y,6)+0.5</f>
         <v>0.5</v>
       </c>
       <c r="D42" s="31">
-        <f>+D40+$K$10</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,14)+Hght_WinWall2</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1658,16 +1678,16 @@
         <v>26</v>
       </c>
       <c r="B43" s="32">
-        <f>+B29-0.5</f>
+        <f>INDEX(x,3)-0.5</f>
         <v>10.054619841567009</v>
       </c>
       <c r="C43" s="33">
-        <f>+C29</f>
+        <f>INDEX(y,3)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D43" s="33">
-        <f>+D29+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,3)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,16 +1695,16 @@
         <v>27</v>
       </c>
       <c r="B44" s="32">
-        <f>+B43-$J$11</f>
+        <f>INDEX(x,17)-Len_WinWall3</f>
         <v>7.099326285928246</v>
       </c>
       <c r="C44" s="33">
-        <f>+C30</f>
+        <f>INDEX(y,4)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D44" s="33">
-        <f>+D30+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,4)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1692,16 +1712,16 @@
         <v>28</v>
       </c>
       <c r="B45" s="32">
-        <f>+B44</f>
+        <f>INDEX(x,18)</f>
         <v>7.099326285928246</v>
       </c>
       <c r="C45" s="33">
-        <f>+C44</f>
+        <f>INDEX(y,18)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D45" s="33">
-        <f>+D44+$K$11</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,18)+Hght_WinWall3</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1709,16 +1729,16 @@
         <v>29</v>
       </c>
       <c r="B46" s="32">
-        <f>+B43</f>
+        <f>INDEX(x,17)</f>
         <v>10.054619841567009</v>
       </c>
       <c r="C46" s="33">
-        <f>+C45</f>
+        <f>INDEX(y,19)</f>
         <v>10.554619841567009</v>
       </c>
       <c r="D46" s="33">
-        <f>+D45</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,19)</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1726,16 +1746,16 @@
         <v>30</v>
       </c>
       <c r="B47" s="34">
-        <f>+B30</f>
+        <f>INDEX(x,4)</f>
         <v>0</v>
       </c>
       <c r="C47" s="34">
-        <f>+C30-0.5</f>
+        <f>INDEX(y,4)-0.5</f>
         <v>10.054619841567009</v>
       </c>
       <c r="D47" s="34">
-        <f>+D30+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,4)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1743,16 +1763,16 @@
         <v>31</v>
       </c>
       <c r="B48" s="34">
-        <f>+B27</f>
+        <f>INDEX(x,1)</f>
         <v>0</v>
       </c>
       <c r="C48" s="34">
-        <f>+C47-$J$12</f>
+        <f>INDEX(y,21)-Len_WinWall4</f>
         <v>7.099326285928246</v>
       </c>
       <c r="D48" s="34">
-        <f>+D27+0.5</f>
-        <v>2.9384000000000001</v>
+        <f>INDEX(z,1)+0.5</f>
+        <v>3.01</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1760,16 +1780,16 @@
         <v>32</v>
       </c>
       <c r="B49" s="34">
-        <f>+B31</f>
+        <f>INDEX(x,5)</f>
         <v>0</v>
       </c>
       <c r="C49" s="34">
-        <f>+C48</f>
+        <f>INDEX(y,22)</f>
         <v>7.099326285928246</v>
       </c>
       <c r="D49" s="34">
-        <f>+D48+$K$12</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,22)+Hght_WinWall4</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1777,21 +1797,21 @@
         <v>33</v>
       </c>
       <c r="B50" s="34">
-        <f>+B34</f>
+        <f>INDEX(x,8)</f>
         <v>0</v>
       </c>
       <c r="C50" s="34">
-        <f>+C47</f>
+        <f>INDEX(y,21)</f>
         <v>10.054619841567009</v>
       </c>
       <c r="D50" s="34">
-        <f>+D49</f>
-        <v>4.4623999999999997</v>
+        <f>INDEX(z,23)</f>
+        <v>4.4049999999999994</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified "geometry calculation" sheet to reference new values (Julia) added to "Geometry options" sheet
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="60" windowWidth="14430" windowHeight="12885" activeTab="2"/>
+    <workbookView xWindow="8850" yWindow="60" windowWidth="14430" windowHeight="12885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry options" sheetId="4" r:id="rId1"/>
@@ -83,6 +83,7 @@
     <definedName name="main_area" localSheetId="3">'geometry calculation-original'!$I$18</definedName>
     <definedName name="main_area">'geometry calculation'!$I$19</definedName>
     <definedName name="NumberStoreys">'Geometry options'!$D$3</definedName>
+    <definedName name="NumStorey">'Geometry options'!$D$4</definedName>
     <definedName name="NumStoreys" localSheetId="3">'geometry calculation-original'!$C$4</definedName>
     <definedName name="NumStoreys" comment="Number of storeys above grade">'geometry calculation'!$C$6</definedName>
     <definedName name="Opt_Area" localSheetId="3">'geometry calculation-original'!$C$5</definedName>
@@ -146,11 +147,45 @@
     <definedName name="z3rd" localSheetId="3">'geometry calculation-original'!$L$28:$L$51</definedName>
     <definedName name="z3rd">'geometry calculation'!$L$32:$L$55</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>jeffblake</author>
+  </authors>
+  <commentList>
+    <comment ref="L6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jeffblake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Roof slope is 8/12</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Purdy, Julia</author>
@@ -185,7 +220,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Purdy, Julia</author>
@@ -221,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="179">
   <si>
     <t>m²</t>
   </si>
@@ -746,6 +781,18 @@
   </si>
   <si>
     <t>Retro_added_spray_int</t>
+  </si>
+  <si>
+    <t>Roof</t>
+  </si>
+  <si>
+    <t>Basement</t>
+  </si>
+  <si>
+    <t>Ottawa_new_2storey</t>
+  </si>
+  <si>
+    <t>Archetype for Ottawa LEEP session - Sep 2014</t>
   </si>
 </sst>
 </file>
@@ -757,7 +804,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,6 +905,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -928,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1042,9 +1102,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1073,12 +1130,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1092,6 +1143,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1611,11 +1698,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,65 +1710,85 @@
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="47" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="47" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="47" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="47" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="10.42578125" style="47" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11.28515625" style="47" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
+    <col min="19" max="19" width="19.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H1" s="67" t="s">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H1" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-    </row>
-    <row r="2" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+    </row>
+    <row r="2" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="72" t="s">
+      <c r="D2" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="74" t="s">
+      <c r="J2" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="K2" s="74" t="s">
+      <c r="K2" s="73" t="s">
         <v>160</v>
       </c>
-      <c r="L2" s="71" t="s">
+      <c r="L2" s="70" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="71" t="s">
+      <c r="M2" s="70" t="s">
         <v>169</v>
       </c>
-      <c r="N2" s="71" t="s">
+      <c r="N2" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" s="70" t="s">
         <v>147</v>
       </c>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>149</v>
       </c>
@@ -1698,8 +1805,8 @@
       <c r="F3" s="47">
         <v>12</v>
       </c>
-      <c r="G3" s="47">
-        <f>+FloorAreaPerStorey/Width</f>
+      <c r="G3" s="66">
+        <f>+E3/F3</f>
         <v>11.012500000000001</v>
       </c>
       <c r="H3" s="47">
@@ -1714,23 +1821,87 @@
       <c r="K3" s="47">
         <v>15</v>
       </c>
-      <c r="L3" s="69">
+      <c r="L3" s="68">
         <f>3/12</f>
         <v>0.25</v>
       </c>
-      <c r="M3" s="70">
+      <c r="M3" s="69">
         <v>6.8680000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N3" s="85">
+        <v>3.048</v>
+      </c>
+      <c r="O3" s="85">
+        <f>IF(NumberStoreys&gt;1,2.44,0)</f>
+        <v>2.44</v>
+      </c>
+      <c r="P3" s="85">
+        <f>IF(NumberStoreys=3,2.44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="85">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="R3" s="85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>153</v>
       </c>
+      <c r="C4" s="47">
+        <v>250</v>
+      </c>
       <c r="D4" s="47">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E4" s="66">
+        <f>+C4/D4</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="F4" s="66">
+        <v>9</v>
+      </c>
+      <c r="G4" s="66">
+        <f>+E4/F4</f>
+        <v>9.2592592592592595</v>
+      </c>
+      <c r="H4" s="66">
+        <v>15</v>
+      </c>
+      <c r="I4" s="66">
+        <v>5</v>
+      </c>
+      <c r="J4" s="66">
+        <v>15</v>
+      </c>
+      <c r="K4" s="66">
+        <v>5</v>
+      </c>
+      <c r="L4" s="69">
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N4" s="85">
+        <v>3.048</v>
+      </c>
+      <c r="O4" s="85">
+        <f>IF(NumberStoreys&gt;1,2.44,0)</f>
+        <v>2.44</v>
+      </c>
+      <c r="P4" s="85">
+        <f>IF(NumberStoreys=3,2.44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="85">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="R4" s="85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>154</v>
       </c>
@@ -1763,11 +1934,90 @@
       <c r="K5" s="47">
         <v>5</v>
       </c>
-      <c r="L5" s="70">
+      <c r="L5" s="69">
         <f>2/12</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="M5" s="70"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="85">
+        <v>3.048</v>
+      </c>
+      <c r="O5" s="85">
+        <f>IF(NumberStoreys&gt;1,2.44,0)</f>
+        <v>2.44</v>
+      </c>
+      <c r="P5" s="85">
+        <f>IF(NumberStoreys=3,2.44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="85">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="R5" s="85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="91">
+        <f>2396.99/10.76</f>
+        <v>222.76858736059478</v>
+      </c>
+      <c r="D6" s="82">
+        <v>2</v>
+      </c>
+      <c r="E6" s="91">
+        <f>+C6/D6</f>
+        <v>111.38429368029739</v>
+      </c>
+      <c r="F6" s="82">
+        <v>12.9</v>
+      </c>
+      <c r="G6" s="68">
+        <f>+E6/F6</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="H6" s="92">
+        <f>100*10.32/56.9</f>
+        <v>18.13708260105448</v>
+      </c>
+      <c r="I6" s="92">
+        <v>0.05</v>
+      </c>
+      <c r="J6" s="92">
+        <f>100*17/66.99</f>
+        <v>25.37692192864607</v>
+      </c>
+      <c r="K6" s="92">
+        <f>100*2.68/63.28</f>
+        <v>4.2351453855878631</v>
+      </c>
+      <c r="L6" s="82">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M6" s="82">
+        <v>1.5</v>
+      </c>
+      <c r="N6" s="93">
+        <v>2.79</v>
+      </c>
+      <c r="O6" s="93">
+        <v>2.44</v>
+      </c>
+      <c r="P6" s="93">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="93">
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="R6" s="93">
+        <v>1.9</v>
+      </c>
+      <c r="S6" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1775,14 +2025,15 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O55"/>
+  <dimension ref="A2:T55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1806,7 +2057,7 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="F2" s="59"/>
       <c r="G2" s="59"/>
@@ -1830,14 +2081,14 @@
       <c r="A4" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="67" t="s">
         <v>155</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
-      <c r="H4" s="76" t="s">
+      <c r="H4" s="89" t="s">
         <v>89</v>
       </c>
       <c r="I4" s="58" t="s">
@@ -1856,8 +2107,8 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="64">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:O38,2,FALSE)</f>
-        <v>264.3</v>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,2,FALSE)</f>
+        <v>222.76858736059478</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -1868,12 +2119,12 @@
       <c r="G5" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="66" t="s">
+      <c r="H5" s="90"/>
+      <c r="I5" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1881,7 +2132,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="64">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:O38,3,FALSE)</f>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,3,FALSE)</f>
         <v>2</v>
       </c>
       <c r="D6" s="1"/>
@@ -1893,11 +2144,11 @@
       </c>
       <c r="I6" s="33">
         <f>+(INDEX(x1st,2)-INDEX(x1st,1))*(INDEX(z1st,7)-INDEX(z1st,2))</f>
-        <v>36.575999999999993</v>
+        <v>35.991000000000007</v>
       </c>
       <c r="J6" s="33">
         <f>+(INDEX(x2nd,2)-INDEX(x2nd,1))*(INDEX(z2nd,7)-INDEX(z2nd,2))</f>
-        <v>29.279999999999994</v>
+        <v>31.475999999999996</v>
       </c>
       <c r="K6" s="33">
         <f>+(INDEX(x3rd,2)-INDEX(x3rd,1))*(INDEX(z3rd,7)-INDEX(z3rd,2))</f>
@@ -1915,8 +2166,8 @@
         <v>6</v>
       </c>
       <c r="C7" s="11">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:O38,4,FALSE)</f>
-        <v>132.15</v>
+        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,4,FALSE)</f>
+        <v>111.38429368029739</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>0</v>
@@ -1929,11 +2180,11 @@
       </c>
       <c r="I7" s="33">
         <f>+(INDEX(y1st,3)-INDEX(y1st,2))*(INDEX(z1st,7)-(INDEX(z1st,3)))</f>
-        <v>33.566099999999999</v>
+        <v>24.090091423878278</v>
       </c>
       <c r="J7" s="33">
         <f>+(INDEX(y2nd,3)-INDEX(y2nd,2))*(INDEX(z2nd,7)-(INDEX(z2nd,3)))</f>
-        <v>26.870499999999996</v>
+        <v>21.068036944180278</v>
       </c>
       <c r="K7" s="33">
         <f>+(INDEX(y3rd,3)-INDEX(y3rd,2))*(INDEX(z3rd,7)-(INDEX(z3rd,3)))</f>
@@ -1950,9 +2201,9 @@
       <c r="B8" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="79">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:O38,5,FALSE)</f>
-        <v>12</v>
+      <c r="C8" s="76">
+        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,5,FALSE)</f>
+        <v>12.9</v>
       </c>
       <c r="D8" s="39" t="s">
         <v>1</v>
@@ -1965,11 +2216,11 @@
       </c>
       <c r="I8" s="33">
         <f>(INDEX(x1st,3)-INDEX(x1st,4))*(INDEX(z1st,7)-INDEX(z1st,4))</f>
-        <v>36.575999999999993</v>
+        <v>35.991000000000007</v>
       </c>
       <c r="J8" s="33">
         <f>(INDEX(x2nd,3)-INDEX(x2nd,4))*(INDEX(z2nd,7)-INDEX(z2nd,4))</f>
-        <v>29.279999999999994</v>
+        <v>31.475999999999996</v>
       </c>
       <c r="K8" s="33">
         <f>(INDEX(x3rd,3)-INDEX(x3rd,4))*(INDEX(z3rd,7)-INDEX(z3rd,4))</f>
@@ -1986,9 +2237,9 @@
       <c r="B9" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="79">
-        <f>VLOOKUP($B$2,'Geometry options'!B3:O38,6,FALSE)</f>
-        <v>11.012500000000001</v>
+      <c r="C9" s="76">
+        <f>VLOOKUP($B$2,'Geometry options'!B3:S38,6,FALSE)</f>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>1</v>
@@ -2002,11 +2253,11 @@
       </c>
       <c r="I9" s="33">
         <f>(INDEX(y1st,4)-INDEX(y1st,1))*(INDEX(z1st,8)-INDEX(z1st,4))</f>
-        <v>33.566099999999999</v>
+        <v>24.090091423878278</v>
       </c>
       <c r="J9" s="33">
         <f>(INDEX(y2nd,4)-INDEX(y2nd,1))*(INDEX(z2nd,8)-INDEX(z2nd,4))</f>
-        <v>26.870499999999996</v>
+        <v>21.068036944180278</v>
       </c>
       <c r="K9" s="33">
         <f>(INDEX(y3rd,4)-INDEX(y3rd,1))*(INDEX(z3rd,8)-INDEX(z3rd,4))</f>
@@ -2021,8 +2272,9 @@
         <v>72</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="63">
-        <v>3.048</v>
+      <c r="C10" s="76">
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,13,FALSE)</f>
+        <v>2.79</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -2035,15 +2287,15 @@
       </c>
       <c r="I10" s="33">
         <f>INDEX(x1st,6)*INDEX(y1st,7)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="J10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="K10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="L10" t="s">
         <v>0</v>
@@ -2054,8 +2306,8 @@
         <v>73</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="63">
-        <f>IF(NumStoreys&gt;1,2.44,0)</f>
+      <c r="C11" s="76">
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,14,FALSE)</f>
         <v>2.44</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2069,15 +2321,15 @@
       </c>
       <c r="I11" s="33">
         <f>INDEX(x1st,3)*INDEX(y1st,4)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="J11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="K11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="L11" t="s">
         <v>0</v>
@@ -2094,8 +2346,8 @@
         <v>88</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="63">
-        <f>IF(NumStoreys=3,2.44,0)</f>
+      <c r="C12" s="76">
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,15,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2109,34 +2361,34 @@
       </c>
       <c r="H12" s="43">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,7,FALSE)</f>
-        <v>15</v>
+        <v>18.13708260105448</v>
       </c>
       <c r="I12" s="15">
         <f>AreaWall1*AreaWinWall1Ratio/100</f>
-        <v>5.4863999999999988</v>
+        <v>6.5277173989455193</v>
       </c>
       <c r="J12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>4.3919999999999995</v>
+        <v>5.7088281195079071</v>
       </c>
       <c r="K12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>4.3919999999999995</v>
+        <v>5.7088281195079071</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M12" s="27">
         <f>AreaWinWall1/Hght_WinWall1</f>
-        <v>3.5999999999999996</v>
+        <v>4.6793673110720562</v>
       </c>
       <c r="N12" s="26">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O12">
         <f>+Len_WinWall1*Hght_WinWall1</f>
-        <v>5.4863999999999988</v>
+        <v>6.5277173989455193</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2144,7 +2396,8 @@
         <v>31</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="63">
+      <c r="C13" s="76">
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,16,FALSE)</f>
         <v>2.4384000000000001</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2158,34 +2411,34 @@
       </c>
       <c r="H13" s="44">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,8,FALSE)</f>
-        <v>15</v>
+        <v>0.05</v>
       </c>
       <c r="I13" s="17">
         <f>AreaWall2*AreaWinWall2Ratio/100</f>
-        <v>5.0349149999999998</v>
+        <v>1.204504571193914E-2</v>
       </c>
       <c r="J13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>4.0305749999999998</v>
+        <v>1.0534018472090139E-2</v>
       </c>
       <c r="K13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>4.0305749999999998</v>
+        <v>1.0534018472090139E-2</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="M13" s="28">
         <f>AreaWinWall2/Hght_WinWall2</f>
-        <v>3.3037500000000004</v>
+        <v>8.6344413705656906E-3</v>
       </c>
       <c r="N13" s="29">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O13">
         <f>+Len_WinWall2*Hght_WinWall2</f>
-        <v>5.0349149999999998</v>
+        <v>1.204504571193914E-2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2193,8 +2446,9 @@
         <v>74</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="63">
-        <v>2</v>
+      <c r="C14" s="76">
+        <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,17,FALSE)</f>
+        <v>1.9</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -2207,34 +2461,34 @@
       </c>
       <c r="H14" s="45">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,9,FALSE)</f>
-        <v>15</v>
+        <v>25.37692192864607</v>
       </c>
       <c r="I14" s="18">
         <f>AreaWall3*AreaWinWall3Ratio/100</f>
-        <v>5.4863999999999988</v>
+        <v>9.1334079713390093</v>
       </c>
       <c r="J14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>4.3919999999999995</v>
+        <v>7.9876399462606358</v>
       </c>
       <c r="K14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>4.3919999999999995</v>
+        <v>7.9876399462606358</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="M14" s="30">
         <f>AreaWinWall3/Hght_WinWall3</f>
-        <v>3.5999999999999996</v>
+        <v>6.5472458575906867</v>
       </c>
       <c r="N14" s="31">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O14">
         <f>+Len_WinWall3*Hght_WinWall3</f>
-        <v>5.4863999999999988</v>
+        <v>9.1334079713390093</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2244,7 +2498,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="39">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>49</v>
@@ -2254,34 +2508,34 @@
       </c>
       <c r="H15" s="46">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,10,FALSE)</f>
-        <v>15</v>
+        <v>4.2351453855878631</v>
       </c>
       <c r="I15" s="20">
         <f>AreaWall4*AreaWinWall4Ratio/100</f>
-        <v>5.0349149999999998</v>
+        <v>1.0202503953222783</v>
       </c>
       <c r="J15" s="20">
         <f>AreaWall4_2nd*AreaWinWall4Ratio/100</f>
-        <v>4.0305749999999998</v>
+        <v>0.89226199447539722</v>
       </c>
       <c r="K15" s="20">
         <f>AreaWall4_2nd*AreaWinWall4Ratio/100</f>
-        <v>4.0305749999999998</v>
+        <v>0.89226199447539722</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="M15" s="36">
         <f>AreaWinWall4/Hght_WinWall4</f>
-        <v>3.3037500000000004</v>
+        <v>0.73136229055360447</v>
       </c>
       <c r="N15" s="32">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.5239999999999998</v>
+        <v>1.3950000000000002</v>
       </c>
       <c r="O15">
         <f>+Len_WinWall4*Hght_WinWall4</f>
-        <v>5.0349149999999998</v>
+        <v>1.0202503953222783</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2289,54 +2543,54 @@
         <v>148</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="75">
+      <c r="C16" s="74">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,11,FALSE)</f>
-        <v>0.25</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="78"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="61"/>
       <c r="J16" s="61"/>
       <c r="K16" s="61"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="82"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L16" s="77"/>
+      <c r="M16" s="78"/>
+      <c r="N16" s="79"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="7" t="s">
         <v>162</v>
       </c>
       <c r="C17" s="35">
         <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Width*Roof_Slope1)</f>
-        <v>10.926399999999999</v>
+        <v>16.2727</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="78"/>
+      <c r="H17" s="75"/>
       <c r="I17" s="61"/>
       <c r="J17" s="61"/>
       <c r="K17" s="61"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="82"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="77"/>
+      <c r="M17" s="78"/>
+      <c r="N17" s="79"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C18" s="11">
         <f>Opt_Width/2</f>
-        <v>6</v>
+        <v>6.45</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
         <v>55</v>
@@ -2350,19 +2604,19 @@
       </c>
       <c r="I19" s="42">
         <f>SUM(I6:I9)</f>
-        <v>140.2842</v>
+        <v>120.16218284775657</v>
       </c>
       <c r="J19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="15">
         <f>INDEX(x1st,10)</f>
-        <v>4.0999999999999996</v>
+        <v>5.1793673110720562</v>
       </c>
       <c r="D20" s="1"/>
       <c r="F20" t="s">
@@ -2370,7 +2624,7 @@
       </c>
       <c r="I20">
         <f>+SUM(J6:J9)</f>
-        <v>112.30099999999999</v>
+        <v>105.08807388836055</v>
       </c>
       <c r="J20" t="s">
         <v>0</v>
@@ -2378,7 +2632,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="4" t="s">
         <v>57</v>
@@ -2398,96 +2652,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C22" s="17">
         <f>INDEX(y1st,14)</f>
-        <v>3.8037500000000004</v>
+        <v>0.50863444137056568</v>
       </c>
       <c r="F22" t="s">
         <v>136</v>
       </c>
       <c r="I22">
         <f>2*(Opt_Width*Opt_Bsm_Height)+2*(Opt_Length*Opt_Bsm_Height)</f>
-        <v>112.22736</v>
+        <v>105.01916367597477</v>
       </c>
       <c r="J22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="18">
         <f>INDEX(x1st,17)</f>
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="F23" t="s">
         <v>161</v>
       </c>
       <c r="I23">
         <f>+AreaWinWall1Ratio/100*SUM(I6:K6)+AreaWinWall2Ratio/100*SUM(I7:K7)+AreaWinWall3Ratio/100*SUM(I8:K8)+AreaWinWall4Ratio/100*SUM(I9:K9)</f>
-        <v>37.887779999999992</v>
+        <v>31.292684890034774</v>
       </c>
       <c r="J23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="18">
         <f>INDEX(x1st,18)</f>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.8527541424093137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="19">
         <f>INDEX(y1st,21)</f>
-        <v>10.512500000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>8.1344413705656891</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C26" s="20">
         <f>INDEX(y1st,22)</f>
-        <v>7.2087500000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7.4030790800120849</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="61"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="65" t="s">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="F30" s="65" t="s">
+      <c r="C30" s="87"/>
+      <c r="D30" s="87"/>
+      <c r="F30" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="J30" s="65" t="s">
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="J30" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="N30" s="87" t="s">
+        <v>175</v>
+      </c>
+      <c r="O30" s="87"/>
+      <c r="P30" s="87"/>
+      <c r="R30" s="87" t="s">
+        <v>176</v>
+      </c>
+      <c r="S30" s="87"/>
+      <c r="T30" s="87"/>
+    </row>
+    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>54</v>
       </c>
@@ -2518,8 +2782,26 @@
       <c r="L31" s="37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N31" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="O31" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="P31" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="R31" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="S31" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="T31" s="65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -2541,7 +2823,7 @@
       </c>
       <c r="H32" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="J32" s="24">
         <v>0</v>
@@ -2553,14 +2835,33 @@
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N32" s="24">
+        <v>0</v>
+      </c>
+      <c r="O32" s="24">
+        <v>0</v>
+      </c>
+      <c r="P32" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R32" s="24">
+        <v>0</v>
+      </c>
+      <c r="S32" s="24">
+        <v>0</v>
+      </c>
+      <c r="T32" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C33" s="24">
         <v>0</v>
@@ -2571,18 +2872,18 @@
       </c>
       <c r="F33" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G33" s="24">
         <v>0</v>
       </c>
       <c r="H33" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="J33" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K33" s="24">
         <v>0</v>
@@ -2591,18 +2892,39 @@
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N33" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="O33" s="24">
+        <v>0</v>
+      </c>
+      <c r="P33" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R33" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="S33" s="24">
+        <v>0</v>
+      </c>
+      <c r="T33" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C34" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D34" s="24">
         <f>Opt_Bsm_Height</f>
@@ -2610,30 +2932,53 @@
       </c>
       <c r="F34" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G34" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H34" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="J34" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K34" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L34" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N34" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="O34" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P34" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R34" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="S34" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T34" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2642,7 +2987,7 @@
       </c>
       <c r="C35" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D35" s="24">
         <f>Opt_Bsm_Height</f>
@@ -2653,25 +2998,46 @@
       </c>
       <c r="G35" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H35" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="J35" s="24">
         <v>0</v>
       </c>
       <c r="K35" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L35" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N35" s="24">
+        <v>0</v>
+      </c>
+      <c r="O35" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P35" s="24">
+        <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
+        <v>7.6684000000000001</v>
+      </c>
+      <c r="R35" s="24">
+        <v>0</v>
+      </c>
+      <c r="S35" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T35" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2683,7 +3049,7 @@
       </c>
       <c r="D36" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
@@ -2693,7 +3059,7 @@
       </c>
       <c r="H36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
+        <v>7.6684000000000001</v>
       </c>
       <c r="J36" s="24">
         <v>0</v>
@@ -2705,36 +3071,57 @@
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N36" s="25">
+        <f>+Opt_Roof_Peak_W</f>
+        <v>6.45</v>
+      </c>
+      <c r="O36" s="24">
+        <v>0</v>
+      </c>
+      <c r="P36" s="24">
+        <f>+C17</f>
+        <v>16.2727</v>
+      </c>
+      <c r="R36" s="24">
+        <v>0</v>
+      </c>
+      <c r="S36" s="24">
+        <v>0</v>
+      </c>
+      <c r="T36" s="57">
+        <f>Opt_Bsm_Height</f>
+        <v>2.4384000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C37" s="24">
         <v>0</v>
       </c>
       <c r="D37" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="F37" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G37" s="24">
         <v>0</v>
       </c>
       <c r="H37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
+        <v>7.6684000000000001</v>
       </c>
       <c r="J37" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K37" s="24">
         <v>0</v>
@@ -2743,49 +3130,86 @@
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N37" s="25">
+        <f>+Opt_Roof_Peak_W</f>
+        <v>6.45</v>
+      </c>
+      <c r="O37" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="P37" s="24">
+        <f>+C17</f>
+        <v>16.2727</v>
+      </c>
+      <c r="R37" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="S37" s="24">
+        <v>0</v>
+      </c>
+      <c r="T37" s="57">
+        <f>Opt_Bsm_Height</f>
+        <v>2.4384000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C38" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D38" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="F38" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G38" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
+        <v>7.6684000000000001</v>
       </c>
       <c r="J38" s="25">
         <f>Opt_Width</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K38" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L38" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N38" s="83"/>
+      <c r="O38" s="84"/>
+      <c r="R38" s="25">
+        <f>Opt_Width</f>
+        <v>12.9</v>
+      </c>
+      <c r="S38" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T38" s="57">
+        <f>Opt_Bsm_Height</f>
+        <v>2.4384000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2794,36 +3218,49 @@
       </c>
       <c r="C39" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D39" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.4863999999999997</v>
+        <v>5.2284000000000006</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
       </c>
       <c r="G39" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.9263999999999992</v>
+        <v>7.6684000000000001</v>
       </c>
       <c r="J39" s="24">
         <v>0</v>
       </c>
       <c r="K39" s="24">
         <f>Opt_Length</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L39" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N39" s="84"/>
+      <c r="O39" s="84"/>
+      <c r="R39" s="24">
+        <v>0</v>
+      </c>
+      <c r="S39" s="24">
+        <f>Opt_Length</f>
+        <v>8.6344413705656891</v>
+      </c>
+      <c r="T39" s="57">
+        <f>Opt_Bsm_Height</f>
+        <v>2.4384000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>15</v>
       </c>
@@ -2849,7 +3286,7 @@
       </c>
       <c r="H40" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J40" s="26">
         <f>INDEX(x3rd,1)+0.5</f>
@@ -2864,13 +3301,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>4.0999999999999996</v>
+        <v>5.1793673110720562</v>
       </c>
       <c r="C41" s="26">
         <f>INDEX(y1st,2)</f>
@@ -2882,7 +3319,7 @@
       </c>
       <c r="F41" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>4.0999999999999996</v>
+        <v>5.1793673110720562</v>
       </c>
       <c r="G41" s="26">
         <f>INDEX(y2nd,2)</f>
@@ -2890,11 +3327,11 @@
       </c>
       <c r="H41" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J41" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>4.0999999999999996</v>
+        <v>5.1793673110720562</v>
       </c>
       <c r="K41" s="26">
         <f>INDEX(y3rd,2)</f>
@@ -2905,13 +3342,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B42" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>4.0999999999999996</v>
+        <v>5.1793673110720562</v>
       </c>
       <c r="C42" s="26">
         <f>INDEX(y1st,5)</f>
@@ -2919,11 +3356,11 @@
       </c>
       <c r="D42" s="26">
         <f>INDEX(z1st,9)+Hght_WinWall1</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F42" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>4.0999999999999996</v>
+        <v>5.1793673110720562</v>
       </c>
       <c r="G42" s="26">
         <f>INDEX(y2nd,5)</f>
@@ -2931,11 +3368,11 @@
       </c>
       <c r="H42" s="26">
         <f>INDEX(z2nd,9)+Hght_WinWall1</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J42" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>4.0999999999999996</v>
+        <v>5.1793673110720562</v>
       </c>
       <c r="K42" s="26">
         <f>INDEX(y3rd,5)</f>
@@ -2943,10 +3380,10 @@
       </c>
       <c r="L42" s="26">
         <f>INDEX(z3rd,9)+Hght_WinWall1</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.8950000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>18</v>
       </c>
@@ -2960,7 +3397,7 @@
       </c>
       <c r="D43" s="26">
         <f>INDEX(z1st,10)+Hght_WinWall1</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F43" s="26">
         <f>INDEX(x2nd,9)</f>
@@ -2972,7 +3409,7 @@
       </c>
       <c r="H43" s="26">
         <f>INDEX(z2nd,10)+Hght_WinWall1</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J43" s="26">
         <f>INDEX(x3rd,9)</f>
@@ -2984,16 +3421,16 @@
       </c>
       <c r="L43" s="26">
         <f>INDEX(z3rd,10)+Hght_WinWall1</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.8950000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="28">
         <f>INDEX(x1st,2)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C44" s="29">
         <f>INDEX(y1st,2)+0.5</f>
@@ -3005,7 +3442,7 @@
       </c>
       <c r="F44" s="28">
         <f>INDEX(x2nd,2)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G44" s="29">
         <f>INDEX(y2nd,2)+0.5</f>
@@ -3013,11 +3450,11 @@
       </c>
       <c r="H44" s="29">
         <f>INDEX(z2nd,2)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J44" s="28">
         <f>INDEX(x3rd,2)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K44" s="29">
         <f>INDEX(y3rd,2)+0.5</f>
@@ -3028,17 +3465,17 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B45" s="28">
         <f>INDEX(x1st,3)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C45" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>3.8037500000000004</v>
+        <v>0.50863444137056568</v>
       </c>
       <c r="D45" s="29">
         <f>INDEX(z1st,3)+0.5</f>
@@ -3046,77 +3483,77 @@
       </c>
       <c r="F45" s="28">
         <f>INDEX(x2nd,3)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G45" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>3.8037500000000004</v>
+        <v>0.50863444137056568</v>
       </c>
       <c r="H45" s="29">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J45" s="28">
         <f>INDEX(x3rd,3)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K45" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>3.8037500000000004</v>
+        <v>0.50863444137056568</v>
       </c>
       <c r="L45" s="29">
         <f>INDEX(z3rd,3)+0.5</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="28">
         <f>INDEX(x1st,7)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C46" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>3.8037500000000004</v>
+        <v>0.50863444137056568</v>
       </c>
       <c r="D46" s="29">
         <f>INDEX(z1st,13)+Hght_WinWall2</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F46" s="28">
         <f>INDEX(x2nd,7)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G46" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>3.8037500000000004</v>
+        <v>0.50863444137056568</v>
       </c>
       <c r="H46" s="29">
         <f>INDEX(z2nd,13)+Hght_WinWall2</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J46" s="28">
         <f>INDEX(x3rd,7)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K46" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>3.8037500000000004</v>
+        <v>0.50863444137056568</v>
       </c>
       <c r="L46" s="29">
         <f>INDEX(z3rd,13)+Hght_WinWall2</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.8950000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="28">
         <f>INDEX(x1st,6)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="C47" s="29">
         <f>INDEX(y1st,6)+0.5</f>
@@ -3124,11 +3561,11 @@
       </c>
       <c r="D47" s="29">
         <f>INDEX(z1st,14)+Hght_WinWall2</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F47" s="28">
         <f>INDEX(x2nd,6)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="G47" s="29">
         <f>INDEX(y2nd,6)+0.5</f>
@@ -3136,11 +3573,11 @@
       </c>
       <c r="H47" s="29">
         <f>INDEX(z2nd,14)+Hght_WinWall2</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J47" s="28">
         <f>INDEX(x3rd,6)</f>
-        <v>12</v>
+        <v>12.9</v>
       </c>
       <c r="K47" s="29">
         <f>INDEX(y3rd,6)+0.5</f>
@@ -3148,20 +3585,20 @@
       </c>
       <c r="L47" s="29">
         <f>INDEX(z3rd,14)+Hght_WinWall2</f>
-        <v>2.024</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.8950000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="30">
         <f>INDEX(x1st,3)-0.5</f>
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="C48" s="31">
         <f>INDEX(y1st,3)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D48" s="31">
         <f>INDEX(z1st,3)+0.5</f>
@@ -3169,23 +3606,23 @@
       </c>
       <c r="F48" s="30">
         <f>INDEX(x2nd,3)-0.5</f>
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="G48" s="31">
         <f>INDEX(y2nd,3)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H48" s="31">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J48" s="30">
         <f>INDEX(x3rd,3)-0.5</f>
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="K48" s="31">
         <f>INDEX(y3rd,3)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L48" s="31">
         <f>INDEX(z3rd,3)+0.5</f>
@@ -3198,11 +3635,11 @@
       </c>
       <c r="B49" s="30">
         <f>INDEX(x1st,17)-Len_WinWall3</f>
-        <v>7.9</v>
+        <v>5.8527541424093137</v>
       </c>
       <c r="C49" s="31">
         <f>INDEX(y1st,4)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D49" s="31">
         <f>INDEX(z1st,4)+0.5</f>
@@ -3210,23 +3647,23 @@
       </c>
       <c r="F49" s="30">
         <f>INDEX(x2nd,17)-Len_WinWall3</f>
-        <v>7.9</v>
+        <v>5.8527541424093137</v>
       </c>
       <c r="G49" s="31">
         <f>INDEX(y2nd,4)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H49" s="31">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J49" s="30">
         <f>INDEX(x3rd,17)-Len_WinWall3</f>
-        <v>7.9</v>
+        <v>5.8527541424093137</v>
       </c>
       <c r="K49" s="31">
         <f>INDEX(y3rd,4)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L49" s="31">
         <f>INDEX(z3rd,4)+0.5</f>
@@ -3239,39 +3676,39 @@
       </c>
       <c r="B50" s="30">
         <f>INDEX(x1st,18)</f>
-        <v>7.9</v>
+        <v>5.8527541424093137</v>
       </c>
       <c r="C50" s="31">
         <f>INDEX(y1st,18)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D50" s="31">
         <f>INDEX(z1st,18)+Hght_WinWall3</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F50" s="30">
         <f>INDEX(x2nd,18)</f>
-        <v>7.9</v>
+        <v>5.8527541424093137</v>
       </c>
       <c r="G50" s="31">
         <f>INDEX(y2nd,18)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H50" s="31">
         <f>INDEX(z2nd,18)+Hght_WinWall3</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J50" s="30">
         <f>INDEX(x3rd,18)</f>
-        <v>7.9</v>
+        <v>5.8527541424093137</v>
       </c>
       <c r="K50" s="31">
         <f>INDEX(y3rd,18)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L50" s="31">
         <f>INDEX(z3rd,18)+Hght_WinWall3</f>
-        <v>2.024</v>
+        <v>1.8950000000000002</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3280,39 +3717,39 @@
       </c>
       <c r="B51" s="30">
         <f>INDEX(x1st,17)</f>
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="C51" s="31">
         <f>INDEX(y1st,19)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="D51" s="31">
         <f>INDEX(z1st,19)</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F51" s="30">
         <f>INDEX(x2nd,17)</f>
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="G51" s="31">
         <f>INDEX(y2nd,19)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="H51" s="31">
         <f>INDEX(z2nd,19)</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J51" s="30">
         <f>INDEX(x3rd,17)</f>
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="K51" s="31">
         <f>INDEX(y3rd,19)</f>
-        <v>11.012500000000001</v>
+        <v>8.6344413705656891</v>
       </c>
       <c r="L51" s="31">
         <f>INDEX(z3rd,19)</f>
-        <v>2.024</v>
+        <v>1.8950000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3325,7 +3762,7 @@
       </c>
       <c r="C52" s="32">
         <f>INDEX(y1st,4)-0.5</f>
-        <v>10.512500000000001</v>
+        <v>8.1344413705656891</v>
       </c>
       <c r="D52" s="32">
         <f>INDEX(z1st,4)+0.5</f>
@@ -3337,11 +3774,11 @@
       </c>
       <c r="G52" s="32">
         <f>INDEX(y2nd,4)-0.5</f>
-        <v>10.512500000000001</v>
+        <v>8.1344413705656891</v>
       </c>
       <c r="H52" s="32">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J52" s="32">
         <f>INDEX(x3rd,4)</f>
@@ -3349,7 +3786,7 @@
       </c>
       <c r="K52" s="32">
         <f>INDEX(y3rd,4)-0.5</f>
-        <v>10.512500000000001</v>
+        <v>8.1344413705656891</v>
       </c>
       <c r="L52" s="32">
         <f>INDEX(z3rd,4)+0.5</f>
@@ -3366,7 +3803,7 @@
       </c>
       <c r="C53" s="32">
         <f>INDEX(y1st,21)-Len_WinWall4</f>
-        <v>7.2087500000000002</v>
+        <v>7.4030790800120849</v>
       </c>
       <c r="D53" s="32">
         <f>INDEX(z1st,1)+0.5</f>
@@ -3378,11 +3815,11 @@
       </c>
       <c r="G53" s="32">
         <f>INDEX(y2nd,21)-Len_WinWall4</f>
-        <v>7.2087500000000002</v>
+        <v>7.4030790800120849</v>
       </c>
       <c r="H53" s="32">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.9863999999999997</v>
+        <v>5.7284000000000006</v>
       </c>
       <c r="J53" s="32">
         <f>INDEX(x3rd,1)</f>
@@ -3390,7 +3827,7 @@
       </c>
       <c r="K53" s="32">
         <f>INDEX(y3rd,21)-Len_WinWall4</f>
-        <v>7.2087500000000002</v>
+        <v>7.4030790800120849</v>
       </c>
       <c r="L53" s="32">
         <f>INDEX(z3rd,1)+0.5</f>
@@ -3407,11 +3844,11 @@
       </c>
       <c r="C54" s="32">
         <f>INDEX(y1st,22)</f>
-        <v>7.2087500000000002</v>
+        <v>7.4030790800120849</v>
       </c>
       <c r="D54" s="32">
         <f>INDEX(z1st,22)+Hght_WinWall4</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F54" s="32">
         <f>INDEX(x2nd,5)</f>
@@ -3419,11 +3856,11 @@
       </c>
       <c r="G54" s="32">
         <f>INDEX(y2nd,22)</f>
-        <v>7.2087500000000002</v>
+        <v>7.4030790800120849</v>
       </c>
       <c r="H54" s="32">
         <f>INDEX(z2nd,22)+Hght_WinWall4</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J54" s="32">
         <f>INDEX(x3rd,5)</f>
@@ -3431,11 +3868,11 @@
       </c>
       <c r="K54" s="32">
         <f>INDEX(y3rd,22)</f>
-        <v>7.2087500000000002</v>
+        <v>7.4030790800120849</v>
       </c>
       <c r="L54" s="32">
         <f>INDEX(z3rd,22)+Hght_WinWall4</f>
-        <v>2.024</v>
+        <v>1.8950000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3448,11 +3885,11 @@
       </c>
       <c r="C55" s="32">
         <f>INDEX(y1st,21)</f>
-        <v>10.512500000000001</v>
+        <v>8.1344413705656891</v>
       </c>
       <c r="D55" s="32">
         <f>INDEX(z1st,23)</f>
-        <v>4.4623999999999997</v>
+        <v>4.3334000000000001</v>
       </c>
       <c r="F55" s="32">
         <f>INDEX(x2nd,8)</f>
@@ -3460,11 +3897,11 @@
       </c>
       <c r="G55" s="32">
         <f>INDEX(y2nd,21)</f>
-        <v>10.512500000000001</v>
+        <v>8.1344413705656891</v>
       </c>
       <c r="H55" s="32">
         <f>INDEX(z2nd,23)</f>
-        <v>7.5103999999999997</v>
+        <v>7.1234000000000011</v>
       </c>
       <c r="J55" s="32">
         <f>INDEX(x3rd,8)</f>
@@ -3472,20 +3909,22 @@
       </c>
       <c r="K55" s="32">
         <f>INDEX(y3rd,21)</f>
-        <v>10.512500000000001</v>
+        <v>8.1344413705656891</v>
       </c>
       <c r="L55" s="32">
         <f>INDEX(z3rd,23)</f>
-        <v>2.024</v>
+        <v>1.8950000000000002</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="R30:T30"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="J30:L30"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="J30:L55">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -3514,7 +3953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -3540,10 +3979,10 @@
       <c r="D2" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="83" t="s">
+      <c r="E2" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="80" t="s">
         <v>163</v>
       </c>
       <c r="G2" s="53" t="s">
@@ -3611,15 +4050,15 @@
       </c>
       <c r="E7" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>252.58519999999999</v>
+        <v>225.25025673611714</v>
       </c>
       <c r="F7" s="55">
         <f>+E7*10.7639</f>
-        <v>2718.8018342799996</v>
-      </c>
-      <c r="G7" s="84">
+        <v>2424.5712384818912</v>
+      </c>
+      <c r="G7" s="81">
         <f>+D7*F7</f>
-        <v>25943.41128088515</v>
+        <v>23135.797551202755</v>
       </c>
       <c r="H7" t="s">
         <v>143</v>
@@ -3638,7 +4077,7 @@
       </c>
       <c r="E8" s="55"/>
       <c r="F8" s="55"/>
-      <c r="G8" s="84"/>
+      <c r="G8" s="81"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
@@ -3653,7 +4092,7 @@
       </c>
       <c r="E9" s="55"/>
       <c r="F9" s="55"/>
-      <c r="G9" s="84"/>
+      <c r="G9" s="81"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="52" t="s">
@@ -3668,15 +4107,15 @@
       </c>
       <c r="E10" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>252.58519999999999</v>
+        <v>225.25025673611714</v>
       </c>
       <c r="F10" s="55">
         <f>+E10*10.7639</f>
-        <v>2718.8018342799996</v>
-      </c>
-      <c r="G10" s="84">
+        <v>2424.5712384818912</v>
+      </c>
+      <c r="G10" s="81">
         <f>+D10*F10</f>
-        <v>28432.625404714843</v>
+        <v>25355.627218435067</v>
       </c>
       <c r="H10" t="s">
         <v>144</v>
@@ -3695,7 +4134,7 @@
       </c>
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
-      <c r="G11" s="84"/>
+      <c r="G11" s="81"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
@@ -3710,7 +4149,7 @@
       </c>
       <c r="E12" s="55"/>
       <c r="F12" s="55"/>
-      <c r="G12" s="84"/>
+      <c r="G12" s="81"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
@@ -3725,15 +4164,15 @@
       </c>
       <c r="E13" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>252.58519999999999</v>
+        <v>225.25025673611714</v>
       </c>
       <c r="F13" s="55">
         <f>+E13*10.7639</f>
-        <v>2718.8018342799996</v>
-      </c>
-      <c r="G13" s="84">
+        <v>2424.5712384818912</v>
+      </c>
+      <c r="G13" s="81">
         <f>+D13*F13</f>
-        <v>25855.805444002795</v>
+        <v>23057.672477962784</v>
       </c>
       <c r="H13" t="s">
         <v>172</v>
@@ -3752,7 +4191,7 @@
       </c>
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
-      <c r="G14" s="84"/>
+      <c r="G14" s="81"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
@@ -3767,7 +4206,7 @@
       </c>
       <c r="E15" s="55"/>
       <c r="F15" s="55"/>
-      <c r="G15" s="84"/>
+      <c r="G15" s="81"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="52" t="s">
@@ -3782,15 +4221,15 @@
       </c>
       <c r="E16" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>252.58519999999999</v>
+        <v>225.25025673611714</v>
       </c>
       <c r="F16" s="55">
         <f>+E16*10.7639</f>
-        <v>2718.8018342799996</v>
-      </c>
-      <c r="G16" s="84">
+        <v>2424.5712384818912</v>
+      </c>
+      <c r="G16" s="81">
         <f t="shared" ref="G16:G17" si="0">+D16*F16</f>
-        <v>40782.027514199995</v>
+        <v>36368.568577228369</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -3806,15 +4245,15 @@
       </c>
       <c r="E17" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>252.58519999999999</v>
+        <v>225.25025673611714</v>
       </c>
       <c r="F17" s="55">
         <f>+E17*10.7639</f>
-        <v>2718.8018342799996</v>
-      </c>
-      <c r="G17" s="84">
+        <v>2424.5712384818912</v>
+      </c>
+      <c r="G17" s="81">
         <f t="shared" si="0"/>
-        <v>43650.363449365395</v>
+        <v>38926.49123382676</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -3867,15 +4306,15 @@
       </c>
       <c r="E21" s="55">
         <f>found_wall_area</f>
-        <v>112.22736</v>
+        <v>105.01916367597477</v>
       </c>
       <c r="F21" s="55">
         <f>+E21*10.7639</f>
-        <v>1208.0040803039999</v>
-      </c>
-      <c r="G21" s="69">
+        <v>1130.4157758918248</v>
+      </c>
+      <c r="G21" s="68">
         <f>+F21*D21</f>
-        <v>5266.8977901254393</v>
+        <v>4928.6127828883555</v>
       </c>
       <c r="H21" t="s">
         <v>173</v>
@@ -3922,15 +4361,15 @@
       </c>
       <c r="E24" s="55">
         <f>found_wall_area</f>
-        <v>112.22736</v>
+        <v>105.01916367597477</v>
       </c>
       <c r="F24" s="55">
         <f>+E24*10.7639</f>
-        <v>1208.0040803039999</v>
-      </c>
-      <c r="G24" s="69">
+        <v>1130.4157758918248</v>
+      </c>
+      <c r="G24" s="68">
         <f>+F24*D24</f>
-        <v>10751.236314705602</v>
+        <v>10060.700405437243</v>
       </c>
       <c r="H24" t="s">
         <v>174</v>
@@ -3958,15 +4397,15 @@
       </c>
       <c r="E26" s="55">
         <f>+Opt_Area</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="F26" s="55">
         <f>+E26*10.7639</f>
-        <v>1422.4493849999999</v>
-      </c>
-      <c r="G26" s="69">
+        <v>1198.929398745353</v>
+      </c>
+      <c r="G26" s="68">
         <f>+F26*D26</f>
-        <v>1308.6534342</v>
+        <v>1103.0150468457248</v>
       </c>
       <c r="H26" t="s">
         <v>170</v>
@@ -3985,15 +4424,15 @@
       </c>
       <c r="E27" s="55">
         <f>+Opt_Area</f>
-        <v>132.15</v>
+        <v>111.38429368029739</v>
       </c>
       <c r="F27" s="55">
         <f>+E27*10.7639</f>
-        <v>1422.4493849999999</v>
-      </c>
-      <c r="G27" s="69">
+        <v>1198.929398745353</v>
+      </c>
+      <c r="G27" s="68">
         <f>+F27*D27</f>
-        <v>1422.4493849999999</v>
+        <v>1198.929398745353</v>
       </c>
       <c r="H27" t="s">
         <v>171</v>
@@ -4114,21 +4553,21 @@
       <c r="C37" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="D37" s="84">
+      <c r="D37" s="81">
         <f>+'[1]UNIT COSTS'!$H$63</f>
         <v>70.596743144418141</v>
       </c>
       <c r="E37" s="47">
         <f>+'geometry calculation'!$I$23</f>
-        <v>37.887779999999992</v>
+        <v>31.292684890034774</v>
       </c>
       <c r="F37" s="55">
         <f t="shared" ref="F37:F40" si="1">+E37*10.7639</f>
-        <v>407.8202751419999</v>
-      </c>
-      <c r="G37" s="69">
+        <v>336.8313308878453</v>
+      </c>
+      <c r="G37" s="68">
         <f>+D37*F37</f>
-        <v>28790.7832132857</v>
+        <v>23779.194949681732</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -4138,21 +4577,21 @@
       <c r="C38" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="D38" s="84">
+      <c r="D38" s="81">
         <f>+'[1]UNIT COSTS'!$H$64</f>
         <v>70.596743144418141</v>
       </c>
       <c r="E38" s="47">
         <f>+'geometry calculation'!$I$23</f>
-        <v>37.887779999999992</v>
+        <v>31.292684890034774</v>
       </c>
       <c r="F38" s="55">
         <f t="shared" si="1"/>
-        <v>407.8202751419999</v>
-      </c>
-      <c r="G38" s="69">
+        <v>336.8313308878453</v>
+      </c>
+      <c r="G38" s="68">
         <f t="shared" ref="G38:G40" si="2">+D38*F38</f>
-        <v>28790.7832132857</v>
+        <v>23779.194949681732</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -4162,21 +4601,21 @@
       <c r="C39" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="D39" s="84">
+      <c r="D39" s="81">
         <f>+'[1]UNIT COSTS'!$H$65</f>
         <v>78.848804332674945</v>
       </c>
       <c r="E39" s="47">
         <f>+'geometry calculation'!$I$23</f>
-        <v>37.887779999999992</v>
+        <v>31.292684890034774</v>
       </c>
       <c r="F39" s="55">
         <f t="shared" si="1"/>
-        <v>407.8202751419999</v>
-      </c>
-      <c r="G39" s="69">
+        <v>336.8313308878453</v>
+      </c>
+      <c r="G39" s="68">
         <f t="shared" si="2"/>
-        <v>32156.141077569209</v>
+        <v>26558.747702290206</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -4186,21 +4625,21 @@
       <c r="C40" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="D40" s="84">
+      <c r="D40" s="81">
         <f>+'[1]UNIT COSTS'!$H$66</f>
         <v>78.848804332674945</v>
       </c>
       <c r="E40" s="47">
         <f>+'geometry calculation'!$I$23</f>
-        <v>37.887779999999992</v>
+        <v>31.292684890034774</v>
       </c>
       <c r="F40" s="55">
         <f t="shared" si="1"/>
-        <v>407.8202751419999</v>
-      </c>
-      <c r="G40" s="69">
+        <v>336.8313308878453</v>
+      </c>
+      <c r="G40" s="68">
         <f t="shared" si="2"/>
-        <v>32156.141077569209</v>
+        <v>26558.747702290206</v>
       </c>
     </row>
   </sheetData>
@@ -4284,11 +4723,11 @@
       <c r="H3" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="66" t="s">
+      <c r="I3" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -4878,21 +5317,21 @@
       <c r="C25" s="61"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="65" t="s">
+      <c r="B26" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="F26" s="65" t="s">
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="F26" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="J26" s="65" t="s">
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="J26" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">

</xml_diff>

<commit_message>
modifications made to the generic-2storey model, including: - updating new construction costs for the Lighthouse geometry - updates to the DHW loads and reductions
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="60" windowWidth="14430" windowHeight="12885" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="6015" windowWidth="19230" windowHeight="6060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry options" sheetId="4" r:id="rId1"/>
@@ -107,6 +107,7 @@
     <definedName name="third_area" localSheetId="3">'geometry calculation-original'!$I$20</definedName>
     <definedName name="third_area">'geometry calculation'!$I$21</definedName>
     <definedName name="Total_area">'Geometry options'!$C$3</definedName>
+    <definedName name="total_window_area">'geometry calculation'!$I$23</definedName>
     <definedName name="Width">'Geometry options'!$F$3</definedName>
     <definedName name="win_bottom" localSheetId="3">'geometry calculation-original'!$C$15</definedName>
     <definedName name="win_bottom">'geometry calculation'!#REF!</definedName>
@@ -256,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="180">
   <si>
     <t>m²</t>
   </si>
@@ -793,6 +794,9 @@
   </si>
   <si>
     <t>Archetype for Ottawa LEEP session - Sep 2014</t>
+  </si>
+  <si>
+    <t>Base Case for Lighthouse retrofit analysis. Based on EGH database vancouver 1980</t>
   </si>
 </sst>
 </file>
@@ -988,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1157,10 +1161,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1172,15 +1185,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1701,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,12 +1733,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="90" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
     </row>
     <row r="2" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1803,11 +1811,11 @@
         <v>132.15</v>
       </c>
       <c r="F3" s="47">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="G3" s="66">
         <f>+E3/F3</f>
-        <v>11.012500000000001</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H3" s="47">
         <v>15</v>
@@ -1845,6 +1853,9 @@
       <c r="R3" s="85">
         <v>2</v>
       </c>
+      <c r="S3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1961,14 +1972,14 @@
       <c r="B6" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="91">
+      <c r="C6" s="86">
         <f>2396.99/10.76</f>
         <v>222.76858736059478</v>
       </c>
       <c r="D6" s="82">
         <v>2</v>
       </c>
-      <c r="E6" s="91">
+      <c r="E6" s="86">
         <f>+C6/D6</f>
         <v>111.38429368029739</v>
       </c>
@@ -1979,18 +1990,18 @@
         <f>+E6/F6</f>
         <v>8.6344413705656891</v>
       </c>
-      <c r="H6" s="92">
+      <c r="H6" s="87">
         <f>100*10.32/56.9</f>
         <v>18.13708260105448</v>
       </c>
-      <c r="I6" s="92">
+      <c r="I6" s="87">
         <v>0.05</v>
       </c>
-      <c r="J6" s="92">
+      <c r="J6" s="87">
         <f>100*17/66.99</f>
         <v>25.37692192864607</v>
       </c>
-      <c r="K6" s="92">
+      <c r="K6" s="87">
         <f>100*2.68/63.28</f>
         <v>4.2351453855878631</v>
       </c>
@@ -2000,19 +2011,19 @@
       <c r="M6" s="82">
         <v>1.5</v>
       </c>
-      <c r="N6" s="93">
+      <c r="N6" s="88">
         <v>2.79</v>
       </c>
-      <c r="O6" s="93">
+      <c r="O6" s="88">
         <v>2.44</v>
       </c>
-      <c r="P6" s="93">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="93">
+      <c r="P6" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="88">
         <v>2.4384000000000001</v>
       </c>
-      <c r="R6" s="93">
+      <c r="R6" s="88">
         <v>1.9</v>
       </c>
       <c r="S6" t="s">
@@ -2033,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,7 +2068,7 @@
         <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="F2" s="59"/>
       <c r="G2" s="59"/>
@@ -2088,7 +2099,7 @@
       <c r="D4" s="1"/>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
-      <c r="H4" s="89" t="s">
+      <c r="H4" s="92" t="s">
         <v>89</v>
       </c>
       <c r="I4" s="58" t="s">
@@ -2108,7 +2119,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="64">
         <f>VLOOKUP($B$2,'Geometry options'!B3:S38,2,FALSE)</f>
-        <v>222.76858736059478</v>
+        <v>264.3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -2119,12 +2130,12 @@
       <c r="G5" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="90"/>
-      <c r="I5" s="88" t="s">
+      <c r="H5" s="93"/>
+      <c r="I5" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2144,11 +2155,11 @@
       </c>
       <c r="I6" s="33">
         <f>+(INDEX(x1st,2)-INDEX(x1st,1))*(INDEX(z1st,7)-INDEX(z1st,2))</f>
-        <v>35.991000000000007</v>
+        <v>35.051999999999992</v>
       </c>
       <c r="J6" s="33">
         <f>+(INDEX(x2nd,2)-INDEX(x2nd,1))*(INDEX(z2nd,7)-INDEX(z2nd,2))</f>
-        <v>31.475999999999996</v>
+        <v>28.059999999999995</v>
       </c>
       <c r="K6" s="33">
         <f>+(INDEX(x3rd,2)-INDEX(x3rd,1))*(INDEX(z3rd,7)-INDEX(z3rd,2))</f>
@@ -2167,7 +2178,7 @@
       </c>
       <c r="C7" s="11">
         <f>VLOOKUP($B$2,'Geometry options'!B3:S38,4,FALSE)</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>0</v>
@@ -2180,11 +2191,11 @@
       </c>
       <c r="I7" s="33">
         <f>+(INDEX(y1st,3)-INDEX(y1st,2))*(INDEX(z1st,7)-(INDEX(z1st,3)))</f>
-        <v>24.090091423878278</v>
+        <v>35.025495652173909</v>
       </c>
       <c r="J7" s="33">
         <f>+(INDEX(y2nd,3)-INDEX(y2nd,2))*(INDEX(z2nd,7)-(INDEX(z2nd,3)))</f>
-        <v>21.068036944180278</v>
+        <v>28.038782608695648</v>
       </c>
       <c r="K7" s="33">
         <f>+(INDEX(y3rd,3)-INDEX(y3rd,2))*(INDEX(z3rd,7)-(INDEX(z3rd,3)))</f>
@@ -2203,7 +2214,7 @@
       </c>
       <c r="C8" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!B3:S38,5,FALSE)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="D8" s="39" t="s">
         <v>1</v>
@@ -2216,11 +2227,11 @@
       </c>
       <c r="I8" s="33">
         <f>(INDEX(x1st,3)-INDEX(x1st,4))*(INDEX(z1st,7)-INDEX(z1st,4))</f>
-        <v>35.991000000000007</v>
+        <v>35.051999999999992</v>
       </c>
       <c r="J8" s="33">
         <f>(INDEX(x2nd,3)-INDEX(x2nd,4))*(INDEX(z2nd,7)-INDEX(z2nd,4))</f>
-        <v>31.475999999999996</v>
+        <v>28.059999999999995</v>
       </c>
       <c r="K8" s="33">
         <f>(INDEX(x3rd,3)-INDEX(x3rd,4))*(INDEX(z3rd,7)-INDEX(z3rd,4))</f>
@@ -2239,7 +2250,7 @@
       </c>
       <c r="C9" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!B3:S38,6,FALSE)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>1</v>
@@ -2253,11 +2264,11 @@
       </c>
       <c r="I9" s="33">
         <f>(INDEX(y1st,4)-INDEX(y1st,1))*(INDEX(z1st,8)-INDEX(z1st,4))</f>
-        <v>24.090091423878278</v>
+        <v>35.025495652173909</v>
       </c>
       <c r="J9" s="33">
         <f>(INDEX(y2nd,4)-INDEX(y2nd,1))*(INDEX(z2nd,8)-INDEX(z2nd,4))</f>
-        <v>21.068036944180278</v>
+        <v>28.038782608695648</v>
       </c>
       <c r="K9" s="33">
         <f>(INDEX(y3rd,4)-INDEX(y3rd,1))*(INDEX(z3rd,8)-INDEX(z3rd,4))</f>
@@ -2274,7 +2285,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,13,FALSE)</f>
-        <v>2.79</v>
+        <v>3.048</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -2287,15 +2298,15 @@
       </c>
       <c r="I10" s="33">
         <f>INDEX(x1st,6)*INDEX(y1st,7)</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="J10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="K10" s="33">
         <f>INDEX(x2nd,6)*INDEX(y2nd,7)</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="L10" t="s">
         <v>0</v>
@@ -2321,15 +2332,15 @@
       </c>
       <c r="I11" s="33">
         <f>INDEX(x1st,3)*INDEX(y1st,4)</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="J11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="K11" s="33">
         <f>INDEX(x2nd,3)*INDEX(y2nd,4)</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="L11" t="s">
         <v>0</v>
@@ -2361,34 +2372,34 @@
       </c>
       <c r="H12" s="43">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,7,FALSE)</f>
-        <v>18.13708260105448</v>
+        <v>15</v>
       </c>
       <c r="I12" s="15">
         <f>AreaWall1*AreaWinWall1Ratio/100</f>
-        <v>6.5277173989455193</v>
+        <v>5.2577999999999987</v>
       </c>
       <c r="J12" s="15">
         <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>5.7088281195079071</v>
+        <v>4.2089999999999996</v>
       </c>
       <c r="K12" s="15">
-        <f>AreaWall1_2nd*AreaWinWall1Ratio/100</f>
-        <v>5.7088281195079071</v>
+        <f>+IF(NumStoreys=3,AreaWall1_2nd*AreaWinWall1Ratio/100,0)</f>
+        <v>0</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M12" s="27">
         <f>AreaWinWall1/Hght_WinWall1</f>
-        <v>4.6793673110720562</v>
+        <v>3.4499999999999997</v>
       </c>
       <c r="N12" s="26">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.5239999999999998</v>
       </c>
       <c r="O12">
         <f>+Len_WinWall1*Hght_WinWall1</f>
-        <v>6.5277173989455193</v>
+        <v>5.2577999999999987</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2411,34 +2422,34 @@
       </c>
       <c r="H13" s="44">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,8,FALSE)</f>
-        <v>0.05</v>
+        <v>15</v>
       </c>
       <c r="I13" s="17">
         <f>AreaWall2*AreaWinWall2Ratio/100</f>
-        <v>1.204504571193914E-2</v>
+        <v>5.253824347826086</v>
       </c>
       <c r="J13" s="17">
         <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>1.0534018472090139E-2</v>
+        <v>4.2058173913043468</v>
       </c>
       <c r="K13" s="17">
-        <f>AreaWall2_2nd*AreaWinWall2Ratio/100</f>
-        <v>1.0534018472090139E-2</v>
+        <f>+IF(NumStoreys=3,AreaWall2_2nd*AreaWinWall2Ratio/100,0)</f>
+        <v>0</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="M13" s="28">
         <f>AreaWinWall2/Hght_WinWall2</f>
-        <v>8.6344413705656906E-3</v>
+        <v>3.4473913043478257</v>
       </c>
       <c r="N13" s="29">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.5239999999999998</v>
       </c>
       <c r="O13">
         <f>+Len_WinWall2*Hght_WinWall2</f>
-        <v>1.204504571193914E-2</v>
+        <v>5.253824347826086</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2448,7 +2459,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="76">
         <f>VLOOKUP($B$2,'Geometry options'!$B$3:$S$38,17,FALSE)</f>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -2461,34 +2472,34 @@
       </c>
       <c r="H14" s="45">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,9,FALSE)</f>
-        <v>25.37692192864607</v>
+        <v>15</v>
       </c>
       <c r="I14" s="18">
         <f>AreaWall3*AreaWinWall3Ratio/100</f>
-        <v>9.1334079713390093</v>
+        <v>5.2577999999999987</v>
       </c>
       <c r="J14" s="18">
         <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>7.9876399462606358</v>
+        <v>4.2089999999999996</v>
       </c>
       <c r="K14" s="18">
-        <f>AreaWall3_2nd*AreaWinWall3Ratio/100</f>
-        <v>7.9876399462606358</v>
+        <f>+IF(NumStoreys=3,AreaWall3_2nd*AreaWinWall3Ratio/100,0)</f>
+        <v>0</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="M14" s="30">
         <f>AreaWinWall3/Hght_WinWall3</f>
-        <v>6.5472458575906867</v>
+        <v>3.4499999999999997</v>
       </c>
       <c r="N14" s="31">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.5239999999999998</v>
       </c>
       <c r="O14">
         <f>+Len_WinWall3*Hght_WinWall3</f>
-        <v>9.1334079713390093</v>
+        <v>5.2577999999999987</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2498,7 +2509,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="39">
         <f>Hght_Flr1+Opt_Bsm_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>49</v>
@@ -2508,34 +2519,34 @@
       </c>
       <c r="H15" s="46">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,10,FALSE)</f>
-        <v>4.2351453855878631</v>
+        <v>15</v>
       </c>
       <c r="I15" s="20">
         <f>AreaWall4*AreaWinWall4Ratio/100</f>
-        <v>1.0202503953222783</v>
+        <v>5.253824347826086</v>
       </c>
       <c r="J15" s="20">
         <f>AreaWall4_2nd*AreaWinWall4Ratio/100</f>
-        <v>0.89226199447539722</v>
+        <v>4.2058173913043468</v>
       </c>
       <c r="K15" s="20">
-        <f>AreaWall4_2nd*AreaWinWall4Ratio/100</f>
-        <v>0.89226199447539722</v>
+        <f>+IF(NumStoreys=3,AreaWall4_2nd*AreaWinWall4Ratio/100,0)</f>
+        <v>0</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>0</v>
       </c>
       <c r="M15" s="36">
         <f>AreaWinWall4/Hght_WinWall4</f>
-        <v>0.73136229055360447</v>
+        <v>3.4473913043478257</v>
       </c>
       <c r="N15" s="32">
         <f>(Opt_Main_Height-Opt_Bsm_Height)/2</f>
-        <v>1.3950000000000002</v>
+        <v>1.5239999999999998</v>
       </c>
       <c r="O15">
         <f>+Len_WinWall4*Hght_WinWall4</f>
-        <v>1.0202503953222783</v>
+        <v>5.253824347826086</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2545,7 +2556,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="74">
         <f>VLOOKUP($B$2,'Geometry options'!B3:O38,11,FALSE)</f>
-        <v>0.66700000000000004</v>
+        <v>0.25</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2563,8 +2574,8 @@
         <v>162</v>
       </c>
       <c r="C17" s="35">
-        <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Width*Roof_Slope1)</f>
-        <v>16.2727</v>
+        <f>Opt_Main_Height+Hght_Flr2+Hght_Flr3+(Opt_Roof_Peak_W*Roof_Slope1)</f>
+        <v>9.3638999999999992</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -2586,7 +2597,7 @@
       </c>
       <c r="C18" s="11">
         <f>Opt_Width/2</f>
-        <v>6.45</v>
+        <v>5.75</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2603,8 +2614,8 @@
         <v>134</v>
       </c>
       <c r="I19" s="42">
-        <f>SUM(I6:I9)</f>
-        <v>120.16218284775657</v>
+        <f>SUM(I6:I9)-SUM(I12:I15)</f>
+        <v>119.13174260869562</v>
       </c>
       <c r="J19" t="s">
         <v>0</v>
@@ -2616,15 +2627,15 @@
       </c>
       <c r="C20" s="15">
         <f>INDEX(x1st,10)</f>
-        <v>5.1793673110720562</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="D20" s="1"/>
       <c r="F20" t="s">
         <v>137</v>
       </c>
-      <c r="I20">
-        <f>+SUM(J6:J9)</f>
-        <v>105.08807388836055</v>
+      <c r="I20" s="95">
+        <f>+SUM(J6:J9)-SUM(J12:J15)</f>
+        <v>95.367930434782593</v>
       </c>
       <c r="J20" t="s">
         <v>0</v>
@@ -2644,8 +2655,8 @@
       <c r="F21" t="s">
         <v>135</v>
       </c>
-      <c r="I21">
-        <f>+SUM(K6:K9)</f>
+      <c r="I21" s="95">
+        <f>+SUM(K6:K9)-SUM(K12:K15)</f>
         <v>0</v>
       </c>
       <c r="J21" t="s">
@@ -2659,14 +2670,14 @@
       </c>
       <c r="C22" s="17">
         <f>INDEX(y1st,14)</f>
-        <v>0.50863444137056568</v>
+        <v>3.9473913043478257</v>
       </c>
       <c r="F22" t="s">
         <v>136</v>
       </c>
       <c r="I22">
         <f>2*(Opt_Width*Opt_Bsm_Height)+2*(Opt_Length*Opt_Bsm_Height)</f>
-        <v>105.01916367597477</v>
+        <v>112.12399304347827</v>
       </c>
       <c r="J22" t="s">
         <v>0</v>
@@ -2679,17 +2690,21 @@
       </c>
       <c r="C23" s="18">
         <f>INDEX(x1st,17)</f>
-        <v>12.4</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
         <v>161</v>
       </c>
       <c r="I23">
         <f>+AreaWinWall1Ratio/100*SUM(I6:K6)+AreaWinWall2Ratio/100*SUM(I7:K7)+AreaWinWall3Ratio/100*SUM(I8:K8)+AreaWinWall4Ratio/100*SUM(I9:K9)</f>
-        <v>31.292684890034774</v>
+        <v>37.852883478260864</v>
       </c>
       <c r="J23" t="s">
         <v>0</v>
+      </c>
+      <c r="K23" s="95">
+        <f>+SUM(I12:K15)</f>
+        <v>37.852883478260864</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2699,7 +2714,7 @@
       </c>
       <c r="C24" s="18">
         <f>INDEX(x1st,18)</f>
-        <v>5.8527541424093137</v>
+        <v>7.5500000000000007</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -2708,7 +2723,7 @@
       </c>
       <c r="C25" s="19">
         <f>INDEX(y1st,21)</f>
-        <v>8.1344413705656891</v>
+        <v>10.991304347826087</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -2717,7 +2732,7 @@
       </c>
       <c r="C26" s="20">
         <f>INDEX(y1st,22)</f>
-        <v>7.4030790800120849</v>
+        <v>7.5439130434782617</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -2725,31 +2740,31 @@
       <c r="C29" s="61"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="87" t="s">
+      <c r="B30" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="F30" s="87" t="s">
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="F30" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="J30" s="87" t="s">
+      <c r="G30" s="94"/>
+      <c r="H30" s="94"/>
+      <c r="J30" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="N30" s="87" t="s">
+      <c r="K30" s="94"/>
+      <c r="L30" s="94"/>
+      <c r="N30" s="94" t="s">
         <v>175</v>
       </c>
-      <c r="O30" s="87"/>
-      <c r="P30" s="87"/>
-      <c r="R30" s="87" t="s">
+      <c r="O30" s="94"/>
+      <c r="P30" s="94"/>
+      <c r="R30" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="S30" s="87"/>
-      <c r="T30" s="87"/>
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
@@ -2823,7 +2838,7 @@
       </c>
       <c r="H32" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="J32" s="24">
         <v>0</v>
@@ -2843,7 +2858,7 @@
       </c>
       <c r="P32" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="R32" s="24">
         <v>0</v>
@@ -2861,7 +2876,7 @@
       </c>
       <c r="B33" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C33" s="24">
         <v>0</v>
@@ -2872,18 +2887,18 @@
       </c>
       <c r="F33" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G33" s="24">
         <v>0</v>
       </c>
       <c r="H33" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="J33" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K33" s="24">
         <v>0</v>
@@ -2894,18 +2909,18 @@
       </c>
       <c r="N33" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="O33" s="24">
         <v>0</v>
       </c>
       <c r="P33" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="R33" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="S33" s="24">
         <v>0</v>
@@ -2920,11 +2935,11 @@
       </c>
       <c r="B34" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C34" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D34" s="24">
         <f>Opt_Bsm_Height</f>
@@ -2932,23 +2947,23 @@
       </c>
       <c r="F34" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G34" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H34" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="J34" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K34" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L34" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
@@ -2956,23 +2971,23 @@
       </c>
       <c r="N34" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="O34" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="P34" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="R34" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="S34" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="T34" s="24">
         <v>0</v>
@@ -2987,7 +3002,7 @@
       </c>
       <c r="C35" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D35" s="24">
         <f>Opt_Bsm_Height</f>
@@ -2998,18 +3013,18 @@
       </c>
       <c r="G35" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H35" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="J35" s="24">
         <v>0</v>
       </c>
       <c r="K35" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L35" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2,0)</f>
@@ -3020,18 +3035,18 @@
       </c>
       <c r="O35" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="P35" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="R35" s="24">
         <v>0</v>
       </c>
       <c r="S35" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="T35" s="24">
         <v>0</v>
@@ -3049,7 +3064,7 @@
       </c>
       <c r="D36" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
@@ -3059,7 +3074,7 @@
       </c>
       <c r="H36" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="J36" s="24">
         <v>0</v>
@@ -3073,14 +3088,14 @@
       </c>
       <c r="N36" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>5.75</v>
       </c>
       <c r="O36" s="24">
         <v>0</v>
       </c>
       <c r="P36" s="24">
         <f>+C17</f>
-        <v>16.2727</v>
+        <v>9.3638999999999992</v>
       </c>
       <c r="R36" s="24">
         <v>0</v>
@@ -3099,29 +3114,29 @@
       </c>
       <c r="B37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C37" s="24">
         <v>0</v>
       </c>
       <c r="D37" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="F37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G37" s="24">
         <v>0</v>
       </c>
       <c r="H37" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="J37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K37" s="24">
         <v>0</v>
@@ -3132,19 +3147,19 @@
       </c>
       <c r="N37" s="25">
         <f>+Opt_Roof_Peak_W</f>
-        <v>6.45</v>
+        <v>5.75</v>
       </c>
       <c r="O37" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="P37" s="24">
         <f>+C17</f>
-        <v>16.2727</v>
+        <v>9.3638999999999992</v>
       </c>
       <c r="R37" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="S37" s="24">
         <v>0</v>
@@ -3160,35 +3175,35 @@
       </c>
       <c r="B38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D38" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="F38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H38" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="J38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L38" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
@@ -3198,11 +3213,11 @@
       <c r="O38" s="84"/>
       <c r="R38" s="25">
         <f>Opt_Width</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="S38" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="T38" s="57">
         <f>Opt_Bsm_Height</f>
@@ -3218,29 +3233,29 @@
       </c>
       <c r="C39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D39" s="24">
         <f>Opt_Main_Height</f>
-        <v>5.2284000000000006</v>
+        <v>5.4863999999999997</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
       </c>
       <c r="G39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H39" s="24">
         <f>+Opt_Bsm_Height+Hght_Flr1+Hght_Flr2</f>
-        <v>7.6684000000000001</v>
+        <v>7.9263999999999992</v>
       </c>
       <c r="J39" s="24">
         <v>0</v>
       </c>
       <c r="K39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L39" s="24">
         <f>+IF(NumStoreys=3,Opt_Bsm_Height+Hght_Flr1+Hght_Flr2+Hght_Flr3,0)</f>
@@ -3253,7 +3268,7 @@
       </c>
       <c r="S39" s="24">
         <f>Opt_Length</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="T39" s="57">
         <f>Opt_Bsm_Height</f>
@@ -3286,7 +3301,7 @@
       </c>
       <c r="H40" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J40" s="26">
         <f>INDEX(x3rd,1)+0.5</f>
@@ -3307,7 +3322,7 @@
       </c>
       <c r="B41" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>5.1793673110720562</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="C41" s="26">
         <f>INDEX(y1st,2)</f>
@@ -3319,7 +3334,7 @@
       </c>
       <c r="F41" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>5.1793673110720562</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="G41" s="26">
         <f>INDEX(y2nd,2)</f>
@@ -3327,11 +3342,11 @@
       </c>
       <c r="H41" s="26">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J41" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>5.1793673110720562</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="K41" s="26">
         <f>INDEX(y3rd,2)</f>
@@ -3348,7 +3363,7 @@
       </c>
       <c r="B42" s="27">
         <f>INDEX(x1st,9)+Len_WinWall1</f>
-        <v>5.1793673110720562</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="C42" s="26">
         <f>INDEX(y1st,5)</f>
@@ -3356,11 +3371,11 @@
       </c>
       <c r="D42" s="26">
         <f>INDEX(z1st,9)+Hght_WinWall1</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F42" s="27">
         <f>INDEX(x2nd,9)+Len_WinWall1</f>
-        <v>5.1793673110720562</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="G42" s="26">
         <f>INDEX(y2nd,5)</f>
@@ -3368,11 +3383,11 @@
       </c>
       <c r="H42" s="26">
         <f>INDEX(z2nd,9)+Hght_WinWall1</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J42" s="27">
         <f>INDEX(x3rd,9)+Len_WinWall1</f>
-        <v>5.1793673110720562</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="K42" s="26">
         <f>INDEX(y3rd,5)</f>
@@ -3380,7 +3395,7 @@
       </c>
       <c r="L42" s="26">
         <f>INDEX(z3rd,9)+Hght_WinWall1</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -3397,7 +3412,7 @@
       </c>
       <c r="D43" s="26">
         <f>INDEX(z1st,10)+Hght_WinWall1</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F43" s="26">
         <f>INDEX(x2nd,9)</f>
@@ -3409,7 +3424,7 @@
       </c>
       <c r="H43" s="26">
         <f>INDEX(z2nd,10)+Hght_WinWall1</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J43" s="26">
         <f>INDEX(x3rd,9)</f>
@@ -3421,7 +3436,7 @@
       </c>
       <c r="L43" s="26">
         <f>INDEX(z3rd,10)+Hght_WinWall1</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -3430,7 +3445,7 @@
       </c>
       <c r="B44" s="28">
         <f>INDEX(x1st,2)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C44" s="29">
         <f>INDEX(y1st,2)+0.5</f>
@@ -3442,7 +3457,7 @@
       </c>
       <c r="F44" s="28">
         <f>INDEX(x2nd,2)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G44" s="29">
         <f>INDEX(y2nd,2)+0.5</f>
@@ -3450,11 +3465,11 @@
       </c>
       <c r="H44" s="29">
         <f>INDEX(z2nd,2)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J44" s="28">
         <f>INDEX(x3rd,2)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K44" s="29">
         <f>INDEX(y3rd,2)+0.5</f>
@@ -3471,11 +3486,11 @@
       </c>
       <c r="B45" s="28">
         <f>INDEX(x1st,3)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C45" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>0.50863444137056568</v>
+        <v>3.9473913043478257</v>
       </c>
       <c r="D45" s="29">
         <f>INDEX(z1st,3)+0.5</f>
@@ -3483,23 +3498,23 @@
       </c>
       <c r="F45" s="28">
         <f>INDEX(x2nd,3)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G45" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>0.50863444137056568</v>
+        <v>3.9473913043478257</v>
       </c>
       <c r="H45" s="29">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J45" s="28">
         <f>INDEX(x3rd,3)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K45" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>0.50863444137056568</v>
+        <v>3.9473913043478257</v>
       </c>
       <c r="L45" s="29">
         <f>INDEX(z3rd,3)+0.5</f>
@@ -3512,39 +3527,39 @@
       </c>
       <c r="B46" s="28">
         <f>INDEX(x1st,7)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C46" s="29">
         <f>INDEX(y1st,13)+Len_WinWall2</f>
-        <v>0.50863444137056568</v>
+        <v>3.9473913043478257</v>
       </c>
       <c r="D46" s="29">
         <f>INDEX(z1st,13)+Hght_WinWall2</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F46" s="28">
         <f>INDEX(x2nd,7)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G46" s="29">
         <f>INDEX(y2nd,13)+Len_WinWall2</f>
-        <v>0.50863444137056568</v>
+        <v>3.9473913043478257</v>
       </c>
       <c r="H46" s="29">
         <f>INDEX(z2nd,13)+Hght_WinWall2</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J46" s="28">
         <f>INDEX(x3rd,7)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K46" s="29">
         <f>INDEX(y3rd,13)+Len_WinWall2</f>
-        <v>0.50863444137056568</v>
+        <v>3.9473913043478257</v>
       </c>
       <c r="L46" s="29">
         <f>INDEX(z3rd,13)+Hght_WinWall2</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -3553,7 +3568,7 @@
       </c>
       <c r="B47" s="28">
         <f>INDEX(x1st,6)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="C47" s="29">
         <f>INDEX(y1st,6)+0.5</f>
@@ -3561,11 +3576,11 @@
       </c>
       <c r="D47" s="29">
         <f>INDEX(z1st,14)+Hght_WinWall2</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F47" s="28">
         <f>INDEX(x2nd,6)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="G47" s="29">
         <f>INDEX(y2nd,6)+0.5</f>
@@ -3573,11 +3588,11 @@
       </c>
       <c r="H47" s="29">
         <f>INDEX(z2nd,14)+Hght_WinWall2</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J47" s="28">
         <f>INDEX(x3rd,6)</f>
-        <v>12.9</v>
+        <v>11.5</v>
       </c>
       <c r="K47" s="29">
         <f>INDEX(y3rd,6)+0.5</f>
@@ -3585,7 +3600,7 @@
       </c>
       <c r="L47" s="29">
         <f>INDEX(z3rd,14)+Hght_WinWall2</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -3594,11 +3609,11 @@
       </c>
       <c r="B48" s="30">
         <f>INDEX(x1st,3)-0.5</f>
-        <v>12.4</v>
+        <v>11</v>
       </c>
       <c r="C48" s="31">
         <f>INDEX(y1st,3)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D48" s="31">
         <f>INDEX(z1st,3)+0.5</f>
@@ -3606,23 +3621,23 @@
       </c>
       <c r="F48" s="30">
         <f>INDEX(x2nd,3)-0.5</f>
-        <v>12.4</v>
+        <v>11</v>
       </c>
       <c r="G48" s="31">
         <f>INDEX(y2nd,3)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H48" s="31">
         <f>INDEX(z2nd,3)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J48" s="30">
         <f>INDEX(x3rd,3)-0.5</f>
-        <v>12.4</v>
+        <v>11</v>
       </c>
       <c r="K48" s="31">
         <f>INDEX(y3rd,3)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L48" s="31">
         <f>INDEX(z3rd,3)+0.5</f>
@@ -3635,11 +3650,11 @@
       </c>
       <c r="B49" s="30">
         <f>INDEX(x1st,17)-Len_WinWall3</f>
-        <v>5.8527541424093137</v>
+        <v>7.5500000000000007</v>
       </c>
       <c r="C49" s="31">
         <f>INDEX(y1st,4)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D49" s="31">
         <f>INDEX(z1st,4)+0.5</f>
@@ -3647,23 +3662,23 @@
       </c>
       <c r="F49" s="30">
         <f>INDEX(x2nd,17)-Len_WinWall3</f>
-        <v>5.8527541424093137</v>
+        <v>7.5500000000000007</v>
       </c>
       <c r="G49" s="31">
         <f>INDEX(y2nd,4)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H49" s="31">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J49" s="30">
         <f>INDEX(x3rd,17)-Len_WinWall3</f>
-        <v>5.8527541424093137</v>
+        <v>7.5500000000000007</v>
       </c>
       <c r="K49" s="31">
         <f>INDEX(y3rd,4)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L49" s="31">
         <f>INDEX(z3rd,4)+0.5</f>
@@ -3676,39 +3691,39 @@
       </c>
       <c r="B50" s="30">
         <f>INDEX(x1st,18)</f>
-        <v>5.8527541424093137</v>
+        <v>7.5500000000000007</v>
       </c>
       <c r="C50" s="31">
         <f>INDEX(y1st,18)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D50" s="31">
         <f>INDEX(z1st,18)+Hght_WinWall3</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F50" s="30">
         <f>INDEX(x2nd,18)</f>
-        <v>5.8527541424093137</v>
+        <v>7.5500000000000007</v>
       </c>
       <c r="G50" s="31">
         <f>INDEX(y2nd,18)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H50" s="31">
         <f>INDEX(z2nd,18)+Hght_WinWall3</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J50" s="30">
         <f>INDEX(x3rd,18)</f>
-        <v>5.8527541424093137</v>
+        <v>7.5500000000000007</v>
       </c>
       <c r="K50" s="31">
         <f>INDEX(y3rd,18)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L50" s="31">
         <f>INDEX(z3rd,18)+Hght_WinWall3</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3717,39 +3732,39 @@
       </c>
       <c r="B51" s="30">
         <f>INDEX(x1st,17)</f>
-        <v>12.4</v>
+        <v>11</v>
       </c>
       <c r="C51" s="31">
         <f>INDEX(y1st,19)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="D51" s="31">
         <f>INDEX(z1st,19)</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F51" s="30">
         <f>INDEX(x2nd,17)</f>
-        <v>12.4</v>
+        <v>11</v>
       </c>
       <c r="G51" s="31">
         <f>INDEX(y2nd,19)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="H51" s="31">
         <f>INDEX(z2nd,19)</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J51" s="30">
         <f>INDEX(x3rd,17)</f>
-        <v>12.4</v>
+        <v>11</v>
       </c>
       <c r="K51" s="31">
         <f>INDEX(y3rd,19)</f>
-        <v>8.6344413705656891</v>
+        <v>11.491304347826087</v>
       </c>
       <c r="L51" s="31">
         <f>INDEX(z3rd,19)</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3762,7 +3777,7 @@
       </c>
       <c r="C52" s="32">
         <f>INDEX(y1st,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>10.991304347826087</v>
       </c>
       <c r="D52" s="32">
         <f>INDEX(z1st,4)+0.5</f>
@@ -3774,11 +3789,11 @@
       </c>
       <c r="G52" s="32">
         <f>INDEX(y2nd,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>10.991304347826087</v>
       </c>
       <c r="H52" s="32">
         <f>INDEX(z2nd,4)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J52" s="32">
         <f>INDEX(x3rd,4)</f>
@@ -3786,7 +3801,7 @@
       </c>
       <c r="K52" s="32">
         <f>INDEX(y3rd,4)-0.5</f>
-        <v>8.1344413705656891</v>
+        <v>10.991304347826087</v>
       </c>
       <c r="L52" s="32">
         <f>INDEX(z3rd,4)+0.5</f>
@@ -3803,7 +3818,7 @@
       </c>
       <c r="C53" s="32">
         <f>INDEX(y1st,21)-Len_WinWall4</f>
-        <v>7.4030790800120849</v>
+        <v>7.5439130434782617</v>
       </c>
       <c r="D53" s="32">
         <f>INDEX(z1st,1)+0.5</f>
@@ -3815,11 +3830,11 @@
       </c>
       <c r="G53" s="32">
         <f>INDEX(y2nd,21)-Len_WinWall4</f>
-        <v>7.4030790800120849</v>
+        <v>7.5439130434782617</v>
       </c>
       <c r="H53" s="32">
         <f>INDEX(z2nd,1)+0.5</f>
-        <v>5.7284000000000006</v>
+        <v>5.9863999999999997</v>
       </c>
       <c r="J53" s="32">
         <f>INDEX(x3rd,1)</f>
@@ -3827,7 +3842,7 @@
       </c>
       <c r="K53" s="32">
         <f>INDEX(y3rd,21)-Len_WinWall4</f>
-        <v>7.4030790800120849</v>
+        <v>7.5439130434782617</v>
       </c>
       <c r="L53" s="32">
         <f>INDEX(z3rd,1)+0.5</f>
@@ -3844,11 +3859,11 @@
       </c>
       <c r="C54" s="32">
         <f>INDEX(y1st,22)</f>
-        <v>7.4030790800120849</v>
+        <v>7.5439130434782617</v>
       </c>
       <c r="D54" s="32">
         <f>INDEX(z1st,22)+Hght_WinWall4</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F54" s="32">
         <f>INDEX(x2nd,5)</f>
@@ -3856,11 +3871,11 @@
       </c>
       <c r="G54" s="32">
         <f>INDEX(y2nd,22)</f>
-        <v>7.4030790800120849</v>
+        <v>7.5439130434782617</v>
       </c>
       <c r="H54" s="32">
         <f>INDEX(z2nd,22)+Hght_WinWall4</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J54" s="32">
         <f>INDEX(x3rd,5)</f>
@@ -3868,11 +3883,11 @@
       </c>
       <c r="K54" s="32">
         <f>INDEX(y3rd,22)</f>
-        <v>7.4030790800120849</v>
+        <v>7.5439130434782617</v>
       </c>
       <c r="L54" s="32">
         <f>INDEX(z3rd,22)+Hght_WinWall4</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3885,11 +3900,11 @@
       </c>
       <c r="C55" s="32">
         <f>INDEX(y1st,21)</f>
-        <v>8.1344413705656891</v>
+        <v>10.991304347826087</v>
       </c>
       <c r="D55" s="32">
         <f>INDEX(z1st,23)</f>
-        <v>4.3334000000000001</v>
+        <v>4.4623999999999997</v>
       </c>
       <c r="F55" s="32">
         <f>INDEX(x2nd,8)</f>
@@ -3897,11 +3912,11 @@
       </c>
       <c r="G55" s="32">
         <f>INDEX(y2nd,21)</f>
-        <v>8.1344413705656891</v>
+        <v>10.991304347826087</v>
       </c>
       <c r="H55" s="32">
         <f>INDEX(z2nd,23)</f>
-        <v>7.1234000000000011</v>
+        <v>7.5103999999999997</v>
       </c>
       <c r="J55" s="32">
         <f>INDEX(x3rd,8)</f>
@@ -3909,11 +3924,11 @@
       </c>
       <c r="K55" s="32">
         <f>INDEX(y3rd,21)</f>
-        <v>8.1344413705656891</v>
+        <v>10.991304347826087</v>
       </c>
       <c r="L55" s="32">
         <f>INDEX(z3rd,23)</f>
-        <v>1.8950000000000002</v>
+        <v>2.024</v>
       </c>
     </row>
   </sheetData>
@@ -3936,7 +3951,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Geometry options'!$B$3:$B$30</xm:f>
@@ -3953,8 +3968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4049,16 +4064,16 @@
         <v>9.5422222222222217</v>
       </c>
       <c r="E7" s="55">
-        <f>(main_area+second_area+third_area)</f>
-        <v>225.25025673611714</v>
+        <f>+main_area+second_area+third_area</f>
+        <v>214.4996730434782</v>
       </c>
       <c r="F7" s="55">
         <f>+E7*10.7639</f>
-        <v>2424.5712384818912</v>
+        <v>2308.8530306726948</v>
       </c>
       <c r="G7" s="81">
         <f>+D7*F7</f>
-        <v>23135.797551202755</v>
+        <v>22031.588697130112</v>
       </c>
       <c r="H7" t="s">
         <v>143</v>
@@ -4107,15 +4122,15 @@
       </c>
       <c r="E10" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>225.25025673611714</v>
+        <v>214.4996730434782</v>
       </c>
       <c r="F10" s="55">
         <f>+E10*10.7639</f>
-        <v>2424.5712384818912</v>
+        <v>2308.8530306726948</v>
       </c>
       <c r="G10" s="81">
         <f>+D10*F10</f>
-        <v>25355.627218435067</v>
+        <v>24145.471916323782</v>
       </c>
       <c r="H10" t="s">
         <v>144</v>
@@ -4164,15 +4179,15 @@
       </c>
       <c r="E13" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>225.25025673611714</v>
+        <v>214.4996730434782</v>
       </c>
       <c r="F13" s="55">
         <f>+E13*10.7639</f>
-        <v>2424.5712384818912</v>
+        <v>2308.8530306726948</v>
       </c>
       <c r="G13" s="81">
         <f>+D13*F13</f>
-        <v>23057.672477962784</v>
+        <v>21957.192321697326</v>
       </c>
       <c r="H13" t="s">
         <v>172</v>
@@ -4221,15 +4236,15 @@
       </c>
       <c r="E16" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>225.25025673611714</v>
+        <v>214.4996730434782</v>
       </c>
       <c r="F16" s="55">
         <f>+E16*10.7639</f>
-        <v>2424.5712384818912</v>
+        <v>2308.8530306726948</v>
       </c>
       <c r="G16" s="81">
         <f t="shared" ref="G16:G17" si="0">+D16*F16</f>
-        <v>36368.568577228369</v>
+        <v>34632.79546009042</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -4245,15 +4260,15 @@
       </c>
       <c r="E17" s="55">
         <f>(main_area+second_area+third_area)</f>
-        <v>225.25025673611714</v>
+        <v>214.4996730434782</v>
       </c>
       <c r="F17" s="55">
         <f>+E17*10.7639</f>
-        <v>2424.5712384818912</v>
+        <v>2308.8530306726948</v>
       </c>
       <c r="G17" s="81">
         <f t="shared" si="0"/>
-        <v>38926.49123382676</v>
+        <v>37068.635407450114</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4306,15 +4321,15 @@
       </c>
       <c r="E21" s="55">
         <f>found_wall_area</f>
-        <v>105.01916367597477</v>
+        <v>112.12399304347827</v>
       </c>
       <c r="F21" s="55">
         <f>+E21*10.7639</f>
-        <v>1130.4157758918248</v>
+        <v>1206.8914487206957</v>
       </c>
       <c r="G21" s="68">
         <f>+F21*D21</f>
-        <v>4928.6127828883555</v>
+        <v>5262.0467164222327</v>
       </c>
       <c r="H21" t="s">
         <v>173</v>
@@ -4361,15 +4376,15 @@
       </c>
       <c r="E24" s="55">
         <f>found_wall_area</f>
-        <v>105.01916367597477</v>
+        <v>112.12399304347827</v>
       </c>
       <c r="F24" s="55">
         <f>+E24*10.7639</f>
-        <v>1130.4157758918248</v>
+        <v>1206.8914487206957</v>
       </c>
       <c r="G24" s="68">
         <f>+F24*D24</f>
-        <v>10060.700405437243</v>
+        <v>10741.333893614195</v>
       </c>
       <c r="H24" t="s">
         <v>174</v>
@@ -4397,15 +4412,15 @@
       </c>
       <c r="E26" s="55">
         <f>+Opt_Area</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="F26" s="55">
         <f>+E26*10.7639</f>
-        <v>1198.929398745353</v>
+        <v>1422.4493849999999</v>
       </c>
       <c r="G26" s="68">
         <f>+F26*D26</f>
-        <v>1103.0150468457248</v>
+        <v>1308.6534342</v>
       </c>
       <c r="H26" t="s">
         <v>170</v>
@@ -4424,15 +4439,15 @@
       </c>
       <c r="E27" s="55">
         <f>+Opt_Area</f>
-        <v>111.38429368029739</v>
+        <v>132.15</v>
       </c>
       <c r="F27" s="55">
         <f>+E27*10.7639</f>
-        <v>1198.929398745353</v>
+        <v>1422.4493849999999</v>
       </c>
       <c r="G27" s="68">
         <f>+F27*D27</f>
-        <v>1198.929398745353</v>
+        <v>1422.4493849999999</v>
       </c>
       <c r="H27" t="s">
         <v>171</v>
@@ -4558,16 +4573,16 @@
         <v>70.596743144418141</v>
       </c>
       <c r="E37" s="47">
-        <f>+'geometry calculation'!$I$23</f>
-        <v>31.292684890034774</v>
+        <f>total_window_area</f>
+        <v>37.852883478260864</v>
       </c>
       <c r="F37" s="55">
         <f t="shared" ref="F37:F40" si="1">+E37*10.7639</f>
-        <v>336.8313308878453</v>
+        <v>407.44465247165209</v>
       </c>
       <c r="G37" s="68">
         <f>+D37*F37</f>
-        <v>23779.194949681732</v>
+        <v>28764.265476107936</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -4581,17 +4596,17 @@
         <f>+'[1]UNIT COSTS'!$H$64</f>
         <v>70.596743144418141</v>
       </c>
-      <c r="E38" s="47">
-        <f>+'geometry calculation'!$I$23</f>
-        <v>31.292684890034774</v>
+      <c r="E38" s="89">
+        <f>total_window_area</f>
+        <v>37.852883478260864</v>
       </c>
       <c r="F38" s="55">
         <f t="shared" si="1"/>
-        <v>336.8313308878453</v>
+        <v>407.44465247165209</v>
       </c>
       <c r="G38" s="68">
         <f t="shared" ref="G38:G40" si="2">+D38*F38</f>
-        <v>23779.194949681732</v>
+        <v>28764.265476107936</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -4605,17 +4620,17 @@
         <f>+'[1]UNIT COSTS'!$H$65</f>
         <v>78.848804332674945</v>
       </c>
-      <c r="E39" s="47">
-        <f>+'geometry calculation'!$I$23</f>
-        <v>31.292684890034774</v>
+      <c r="E39" s="89">
+        <f>total_window_area</f>
+        <v>37.852883478260864</v>
       </c>
       <c r="F39" s="55">
         <f t="shared" si="1"/>
-        <v>336.8313308878453</v>
+        <v>407.44465247165209</v>
       </c>
       <c r="G39" s="68">
         <f t="shared" si="2"/>
-        <v>26558.747702290206</v>
+        <v>32126.523679132039</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -4629,17 +4644,17 @@
         <f>+'[1]UNIT COSTS'!$H$66</f>
         <v>78.848804332674945</v>
       </c>
-      <c r="E40" s="47">
-        <f>+'geometry calculation'!$I$23</f>
-        <v>31.292684890034774</v>
+      <c r="E40" s="89">
+        <f>total_window_area</f>
+        <v>37.852883478260864</v>
       </c>
       <c r="F40" s="55">
         <f t="shared" si="1"/>
-        <v>336.8313308878453</v>
+        <v>407.44465247165209</v>
       </c>
       <c r="G40" s="68">
         <f t="shared" si="2"/>
-        <v>26558.747702290206</v>
+        <v>32126.523679132039</v>
       </c>
     </row>
   </sheetData>
@@ -4723,11 +4738,11 @@
       <c r="H3" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -5317,21 +5332,21 @@
       <c r="C25" s="61"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="F26" s="87" t="s">
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="F26" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="J26" s="87" t="s">
+      <c r="G26" s="94"/>
+      <c r="H26" s="94"/>
+      <c r="J26" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="94"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">

</xml_diff>

<commit_message>
updates to the generic model to allow for the optimization of 2 and 3 storey homes with inset garages
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-2storey/2storey_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6015" windowWidth="19230" windowHeight="6060" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="6015" windowWidth="19230" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry options" sheetId="4" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="181">
   <si>
     <t>m²</t>
   </si>
@@ -797,6 +797,9 @@
   </si>
   <si>
     <t>Base Case for Lighthouse retrofit analysis. Based on EGH database vancouver 1980</t>
+  </si>
+  <si>
+    <t>Vancouver_new_3storey_semi</t>
   </si>
 </sst>
 </file>
@@ -992,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1176,6 +1179,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1188,7 +1195,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1707,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S6"/>
+  <dimension ref="B1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,12 +1739,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="92" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
     </row>
     <row r="2" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2028,6 +2034,49 @@
       </c>
       <c r="S6" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="47">
+        <v>176.5</v>
+      </c>
+      <c r="D7" s="47">
+        <v>3</v>
+      </c>
+      <c r="E7" s="86">
+        <f>+C7/D7</f>
+        <v>58.833333333333336</v>
+      </c>
+      <c r="F7" s="47">
+        <v>7</v>
+      </c>
+      <c r="G7" s="47">
+        <f>+E7/F7</f>
+        <v>8.4047619047619051</v>
+      </c>
+      <c r="H7" s="87">
+        <f>100*10.32/56.9</f>
+        <v>18.13708260105448</v>
+      </c>
+      <c r="I7" s="87">
+        <v>1.05</v>
+      </c>
+      <c r="J7" s="87">
+        <f>100*17/66.99</f>
+        <v>25.37692192864607</v>
+      </c>
+      <c r="K7" s="87">
+        <f>100*2.68/63.28</f>
+        <v>4.2351453855878631</v>
+      </c>
+      <c r="L7" s="90">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M7" s="47">
+        <v>2.2999999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2099,7 +2148,7 @@
       <c r="D4" s="1"/>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
-      <c r="H4" s="92" t="s">
+      <c r="H4" s="94" t="s">
         <v>89</v>
       </c>
       <c r="I4" s="58" t="s">
@@ -2130,12 +2179,12 @@
       <c r="G5" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="93"/>
-      <c r="I5" s="91" t="s">
+      <c r="H5" s="95"/>
+      <c r="I5" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2633,7 +2682,7 @@
       <c r="F20" t="s">
         <v>137</v>
       </c>
-      <c r="I20" s="95">
+      <c r="I20" s="91">
         <f>+SUM(J6:J9)-SUM(J12:J15)</f>
         <v>95.367930434782593</v>
       </c>
@@ -2655,7 +2704,7 @@
       <c r="F21" t="s">
         <v>135</v>
       </c>
-      <c r="I21" s="95">
+      <c r="I21" s="91">
         <f>+SUM(K6:K9)-SUM(K12:K15)</f>
         <v>0</v>
       </c>
@@ -2702,7 +2751,7 @@
       <c r="J23" t="s">
         <v>0</v>
       </c>
-      <c r="K23" s="95">
+      <c r="K23" s="91">
         <f>+SUM(I12:K15)</f>
         <v>37.852883478260864</v>
       </c>
@@ -2740,31 +2789,31 @@
       <c r="C29" s="61"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="F30" s="94" t="s">
+      <c r="C30" s="96"/>
+      <c r="D30" s="96"/>
+      <c r="F30" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="J30" s="94" t="s">
+      <c r="G30" s="96"/>
+      <c r="H30" s="96"/>
+      <c r="J30" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
-      <c r="N30" s="94" t="s">
+      <c r="K30" s="96"/>
+      <c r="L30" s="96"/>
+      <c r="N30" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="O30" s="94"/>
-      <c r="P30" s="94"/>
-      <c r="R30" s="94" t="s">
+      <c r="O30" s="96"/>
+      <c r="P30" s="96"/>
+      <c r="R30" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="S30" s="94"/>
-      <c r="T30" s="94"/>
+      <c r="S30" s="96"/>
+      <c r="T30" s="96"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
@@ -3968,7 +4017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -4738,11 +4787,11 @@
       <c r="H3" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="91" t="s">
+      <c r="I3" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -5332,21 +5381,21 @@
       <c r="C25" s="61"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
-      <c r="F26" s="94" t="s">
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="F26" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="G26" s="94"/>
-      <c r="H26" s="94"/>
-      <c r="J26" s="94" t="s">
+      <c r="G26" s="96"/>
+      <c r="H26" s="96"/>
+      <c r="J26" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="K26" s="94"/>
-      <c r="L26" s="94"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="96"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">

</xml_diff>